<commit_message>
Update data package at: 2025-09-25T17:34:39Z
</commit_message>
<xml_diff>
--- a/data/ppag2026-dadosmg/indicadores_planejamento.xlsx
+++ b/data/ppag2026-dadosmg/indicadores_planejamento.xlsx
@@ -879,17 +879,13 @@
       <c r="I5" s="2" t="n">
         <v>45807</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
         <v>100</v>
@@ -897,11 +893,9 @@
       <c r="O5" t="b">
         <v>0</v>
       </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
@@ -923,10 +917,14 @@
           <t>(NÚMERO DE ÁREAS DE PROCESSOS-CHAVES DO NÍVEL 3 IA-CM INSTITUCIONALIZADOS NA AUGE/QUANTIDADE DE ÁREAS DE PROCESSOS-CHAVES DO NÍVEL 3 IA-CM)*100</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr"/>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>A METODOLOGIA DO IACM PRESSUPÕE AVALIAÇÕES PERIÓDICAS A CADA 2 ANOS, CONFORME PREVISTO ATUALMENTE.</t>
+        </is>
+      </c>
       <c r="W5" t="inlineStr"/>
       <c r="X5" s="2" t="n">
-        <v>45896.69444444445</v>
+        <v>45925.68125</v>
       </c>
       <c r="Y5" t="b">
         <v>0</v>
@@ -1294,7 +1292,7 @@
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" s="2" t="n">
-        <v>45876.64236111111</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y9" t="b">
         <v>0</v>
@@ -1411,7 +1409,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>TAXA DE PERMANÊNCIA HOSPITALAR (TPH)</t>
+          <t>PERCENTUAL DE DOCENTES COM TITULAÇÃO DE MESTRE E/OU DOUTOR.</t>
         </is>
       </c>
       <c r="E11" t="b">
@@ -1419,45 +1417,45 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Dia</t>
+          <t>Percentual</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>44196</v>
+        <v>45504</v>
       </c>
       <c r="J11" t="n">
-        <v>6.95</v>
+        <v>92</v>
       </c>
       <c r="K11" t="b">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>6.95</v>
+        <v>93</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>6.95</v>
+        <v>93</v>
       </c>
       <c r="O11" t="b">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>6.95</v>
+        <v>93</v>
       </c>
       <c r="Q11" t="b">
         <v>0</v>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>HOSPITAL UNIVERSITÁRIO CLEMENTE DE FARIA - HUCF</t>
+          <t>PRÓ-REITORIA DE PÓS-GRADUAÇÃO</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1472,7 +1470,7 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>TAXA DE PERMANÊNCIA HOSPITALAR = (NÚMERO DE PACIENTES POR DIA)/TOTAL DE SAÍDAS</t>
+          <t>(DM+DD)/TD*100, ONDE DM: DOCENTES MESTRES, DD: DOCENTES DOUTORES E TD: TOTAL DE DOCENTES</t>
         </is>
       </c>
       <c r="V11" t="inlineStr"/>
@@ -1485,7 +1483,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>MENOR</t>
+          <t>MAIOR</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1501,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE DOCENTES COM TITULAÇÃO DE MESTRE E/OU DOUTOR.</t>
+          <t>TAXA DE ALUNO FORMADO NOS CURSOS DE EDUCAÇÃO PROFISSIONAL E TECNOLÓGICO DE NÍVEL MÉDIO.</t>
         </is>
       </c>
       <c r="E12" t="b">
@@ -1515,41 +1513,41 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>45504</v>
+        <v>44196</v>
       </c>
       <c r="J12" t="n">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="M12" t="b">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="O12" t="b">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="Q12" t="b">
         <v>0</v>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>PRÓ-REITORIA DE PÓS-GRADUAÇÃO</t>
+          <t>CENTRO DE EDUCAÇÃO PROFISSIONAL E TECNOLÓGICO</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1564,7 +1562,7 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>(DM+DD)/TD*100, ONDE DM: DOCENTES MESTRES, DD: DOCENTES DOUTORES E TD: TOTAL DE DOCENTES</t>
+          <t>SOMATÓRIA DO N° DE ALUNOS FORMADOS NOS CURSOS TÉCNICOS X 100 = TOTAL DE ALUNOS MATRICULADOS EM CURSOS TÉCNICOS</t>
         </is>
       </c>
       <c r="V12" t="inlineStr"/>
@@ -1595,7 +1593,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TAXA DE ALUNO FORMADO NOS CURSOS DE EDUCAÇÃO PROFISSIONAL E TECNOLÓGICO DE NÍVEL MÉDIO.</t>
+          <t>TAXA DE OCUPAÇÃO HOSPITALAR (TOH)</t>
         </is>
       </c>
       <c r="E13" t="b">
@@ -1607,7 +1605,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1616,32 +1614,32 @@
         <v>44196</v>
       </c>
       <c r="J13" t="n">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="M13" t="b">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="O13" t="b">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="Q13" t="b">
         <v>0</v>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>CENTRO DE EDUCAÇÃO PROFISSIONAL E TECNOLÓGICO</t>
+          <t>HOSPITAL UNIVERSITÁRIO CLEMENTE DE FARIA - HUCF</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1651,12 +1649,12 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Municipal</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>SOMATÓRIA DO N° DE ALUNOS FORMADOS NOS CURSOS TÉCNICOS X 100 = TOTAL DE ALUNOS MATRICULADOS EM CURSOS TÉCNICOS</t>
+          <t>TAXA DE OCUPAÇÃO HOSPITALAR (TOH)= ((NÚMEROS DE PACIENTES POR DIA INTERNADOS NO PERÍODO) / (NÚMERO DE LEITOS/DIA DISPONÍVEL NO PERÍODO)) * 100</t>
         </is>
       </c>
       <c r="V13" t="inlineStr"/>
@@ -1687,7 +1685,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>TAXA DE OCUPAÇÃO HOSPITALAR (TOH)</t>
+          <t>TAXA DE OCUPAÇÃO DE VAGAS DE RESIDENTES (R1) NOS PROGRAMAS DE RESIDÊNCIA MÉDICA</t>
         </is>
       </c>
       <c r="E14" t="b">
@@ -1699,34 +1697,34 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>44196</v>
+        <v>43830</v>
       </c>
       <c r="J14" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="K14" t="b">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="O14" t="b">
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="Q14" t="b">
         <v>0</v>
@@ -1748,7 +1746,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>TAXA DE OCUPAÇÃO HOSPITALAR (TOH)= ((NÚMEROS DE PACIENTES POR DIA INTERNADOS NO PERÍODO) / (NÚMERO DE LEITOS/DIA DISPONÍVEL NO PERÍODO)) * 100</t>
+          <t>TAXA DE OCUPAÇÃO DE VAGAS RESIDENTES (R1) = (NÚMEROS DE VAGAS OCUPADAS POR RESIDENTES R1 POR PERÍODO)/ (NÚMERO DE VAGAS DISPONIBILIZADAS POR PERÍODO)) *100</t>
         </is>
       </c>
       <c r="V14" t="inlineStr"/>
@@ -1779,7 +1777,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>TAXA DE OCUPAÇÃO DE VAGAS DE RESIDENTES (R1) NOS PROGRAMAS DE RESIDÊNCIA MÉDICA</t>
+          <t>TAXA DE PERMANÊNCIA HOSPITALAR (TPH)</t>
         </is>
       </c>
       <c r="E15" t="b">
@@ -1787,38 +1785,38 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Percentual</t>
+          <t>Dia</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>43830</v>
+        <v>44196</v>
       </c>
       <c r="J15" t="n">
-        <v>100</v>
+        <v>6.95</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>100</v>
+        <v>6.95</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>100</v>
+        <v>6.95</v>
       </c>
       <c r="O15" t="b">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>100</v>
+        <v>6.95</v>
       </c>
       <c r="Q15" t="b">
         <v>0</v>
@@ -1835,12 +1833,12 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Municipal</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>TAXA DE OCUPAÇÃO DE VAGAS RESIDENTES (R1) = (NÚMEROS DE VAGAS OCUPADAS POR RESIDENTES R1 POR PERÍODO)/ (NÚMERO DE VAGAS DISPONIBILIZADAS POR PERÍODO)) *100</t>
+          <t>TAXA DE PERMANÊNCIA HOSPITALAR = (NÚMERO DE PACIENTES POR DIA)/TOTAL DE SAÍDAS</t>
         </is>
       </c>
       <c r="V15" t="inlineStr"/>
@@ -1853,7 +1851,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>MAIOR</t>
+          <t>MENOR</t>
         </is>
       </c>
     </row>
@@ -2954,7 +2952,7 @@
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
       <c r="X27" s="2" t="n">
-        <v>45891.45138888889</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y27" t="b">
         <v>0</v>
@@ -3046,7 +3044,7 @@
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
       <c r="X28" s="2" t="n">
-        <v>45891.45138888889</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y28" t="b">
         <v>0</v>
@@ -3811,7 +3809,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>CAPACITAÇÃO EM GEOTECNOLOGIAS</t>
+          <t>INCREMENTO DE ABRANGÊNCIA DOS PROGRAMAS, PROJETOS E AÇÕES INSTITUCIONAIS DE EDUCAÇÃO AMBIENTAL</t>
         </is>
       </c>
       <c r="E37" t="b">
@@ -3822,42 +3820,38 @@
           <t>Percentual</t>
         </is>
       </c>
-      <c r="G37" t="n">
-        <v>18.5</v>
-      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="2" t="n">
-        <v>45657</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
       <c r="J37" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="K37" t="b">
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="M37" t="b">
         <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="O37" t="b">
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="Q37" t="b">
         <v>0</v>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>DIRETORIA DE ESTRATÉGIAS EM GEOTECNOLOGIAS E INFORMAÇÃO GEOGRÁFICA</t>
+          <t>DIRETORIA DE EDUCAÇÃO AMBIENTAL</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -3867,7 +3861,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>Estadual</t>
+          <t>Municipal</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
@@ -3876,7 +3870,11 @@
         </is>
       </c>
       <c r="V37" t="inlineStr"/>
-      <c r="W37" t="inlineStr"/>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>OS PRODUTOS DO INDICADOR” FORAM REFORMULADOS NO ANO DE 2025. PORTANTO, A NOVA METODOLOGIA ESTÁ EM APURAÇÃO E SERÁ APLICADA A PARTIR DE DEZEMBRO DE 2025. CUMPRE ESCLARECER, QUE EM RELAÇÃO AO PRODUTO DO AMBIENTAÇÃO, O SISTEMA INTEGRADO DE GESTÃO DO AMBIENTAÇÃO – SIGA 3.0 PASSOU POR REESTRUTURAÇÃO, QUE ESTÁ SENDO IMPLEMENTADO A PARTIR DE JANEIRO DE 2025.</t>
+        </is>
+      </c>
       <c r="X37" s="2" t="n">
         <v>45923.42152777778</v>
       </c>
@@ -3903,47 +3901,53 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PROJETOS DE PAGAMENTO POR SERVIÇOS AMBIENTAIS FOMENTADOS, FORTALECIDOS E/OU IMPLEMENTADOS</t>
+          <t>CAPACITAÇÃO EM GEOTECNOLOGIAS</t>
         </is>
       </c>
       <c r="E38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>Percentual</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>18.5</v>
+      </c>
       <c r="H38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>45657</v>
+      </c>
       <c r="J38" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K38" t="b">
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="M38" t="b">
         <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="O38" t="b">
         <v>0</v>
       </c>
-      <c r="P38" t="inlineStr"/>
+      <c r="P38" t="n">
+        <v>17</v>
+      </c>
       <c r="Q38" t="b">
         <v>0</v>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>DPAI – DIRETORIA DE PROJETOS AMBIENTAIS E INSTRUMENTOS ECONÔMICOS</t>
+          <t>DIRETORIA DE ESTRATÉGIAS EM GEOTECNOLOGIAS E INFORMAÇÃO GEOGRÁFICA</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -3958,7 +3962,7 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>PROPORÇÃO DE MUNICÍPIOS QUE IMPLEMENTARAM, FORTALECERAM OU FORAM BENEFICIADOS POR POLÍTICAS PÚBLICAS DE PAGAMENTO POR SERVIÇOS AMBIENTAIS (PSA) EM RELAÇÃO AO TOTAL DE MUNICÍPIOS MINEIROS</t>
+          <t>ÍNDICE = 100 X (NÚMERO DE PRODUTOS DO ANO ATUAL – NÚMERO DE PRODUTOS DO ANO ANTERIOR)/ NÚMERO DE PRODUTOS DO ANO ANTERIOR</t>
         </is>
       </c>
       <c r="V38" t="inlineStr"/>
@@ -3989,11 +3993,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>INCREMENTO DE ABRANGÊNCIA DOS PROGRAMAS, PROJETOS E AÇÕES INSTITUCIONAIS DE EDUCAÇÃO AMBIENTAL</t>
+          <t>PROJETOS DE PAGAMENTO POR SERVIÇOS AMBIENTAIS FOMENTADOS, FORTALECIDOS E/OU IMPLEMENTADOS</t>
         </is>
       </c>
       <c r="E39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -4006,7 +4010,7 @@
       </c>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K39" t="b">
         <v>0</v>
@@ -4023,15 +4027,13 @@
       <c r="O39" t="b">
         <v>0</v>
       </c>
-      <c r="P39" t="n">
-        <v>5</v>
-      </c>
+      <c r="P39" t="inlineStr"/>
       <c r="Q39" t="b">
         <v>0</v>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>DIRETORIA DE EDUCAÇÃO AMBIENTAL</t>
+          <t>DPAI – DIRETORIA DE PROJETOS AMBIENTAIS E INSTRUMENTOS ECONÔMICOS</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -4041,20 +4043,16 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>Municipal</t>
+          <t>Estadual</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>ÍNDICE = 100 X (NÚMERO DE PRODUTOS DO ANO ATUAL – NÚMERO DE PRODUTOS DO ANO ANTERIOR)/ NÚMERO DE PRODUTOS DO ANO ANTERIOR</t>
+          <t>PROPORÇÃO DE MUNICÍPIOS QUE IMPLEMENTARAM, FORTALECERAM OU FORAM BENEFICIADOS POR POLÍTICAS PÚBLICAS DE PAGAMENTO POR SERVIÇOS AMBIENTAIS (PSA) EM RELAÇÃO AO TOTAL DE MUNICÍPIOS MINEIROS</t>
         </is>
       </c>
       <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>OS PRODUTOS DO INDICADOR” FORAM REFORMULADOS NO ANO DE 2025. PORTANTO, A NOVA METODOLOGIA ESTÁ EM APURAÇÃO E SERÁ APLICADA A PARTIR DE DEZEMBRO DE 2025. CUMPRE ESCLARECER, QUE EM RELAÇÃO AO PRODUTO DO AMBIENTAÇÃO, O SISTEMA INTEGRADO DE GESTÃO DO AMBIENTAÇÃO – SIGA 3.0 PASSOU POR REESTRUTURAÇÃO, QUE ESTÁ SENDO IMPLEMENTADO A PARTIR DE JANEIRO DE 2025.</t>
-        </is>
-      </c>
+      <c r="W39" t="inlineStr"/>
       <c r="X39" s="2" t="n">
         <v>45923.42152777778</v>
       </c>
@@ -4815,11 +4813,11 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ÍNDICE DE COBERTURA EM CONSULTA MÉDICA</t>
+          <t xml:space="preserve">ÍNDICE DE COBERTURA EM CONSULTA MÉDICA				</t>
         </is>
       </c>
       <c r="E48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -4827,7 +4825,7 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>1.86</v>
+        <v>1.47</v>
       </c>
       <c r="H48" t="b">
         <v>0</v>
@@ -4836,32 +4834,30 @@
         <v>45657</v>
       </c>
       <c r="J48" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K48" t="b">
         <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="M48" t="b">
         <v>0</v>
       </c>
       <c r="N48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O48" t="b">
         <v>0</v>
       </c>
-      <c r="P48" t="n">
-        <v>3</v>
-      </c>
+      <c r="P48" t="inlineStr"/>
       <c r="Q48" t="b">
         <v>0</v>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>SISTEMA DE CADASTRO DOS BENEFICIÁRIOS (SICAD) E SISTEMA DE AUTORIZAÇÃO E FATURAMENTO ELETRÔNICO (SAFE) DO IPSEMG</t>
+          <t xml:space="preserve">SISTEMA DE CADASTRO ÚNICO (CADU) E SISTEMA DE AUTORIZAÇÃO E FATURAMENTO ELETRÔNICO (SAFE) DO IPSEMG				</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
@@ -4876,7 +4872,7 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>[TOTAL ANUAL DE CONSULTAS MÉDICAS (ELETIVAS, DE URGÊNCIA E DE PRONTO SOCORRO) REALIZADAS / MÉDIA ANUAL DO NÚMERO MENSAL DE BENEFICIÁRIOS ATIVOS NO SISTEMA DE CADASTRO DOS BENEFICIÁRIOS (SICAD)]</t>
+          <t xml:space="preserve">[TOTAL DE CONSULTAS MÉDICAS (ELETIVAS, DE ATENÇÃO PRIMÁRIA, DE URGÊNCIA E DE PRONTO SOCORRO) REALIZADAS / TOTAL DE BENEFICIÁRIOS ATIVOS NO SISTEMA DE CADASTRO ÚNICO (CADU) DO IPSEMG]				</t>
         </is>
       </c>
       <c r="V48" t="inlineStr"/>
@@ -4885,7 +4881,7 @@
         <v>45924.50972222222</v>
       </c>
       <c r="Y48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
@@ -4907,11 +4903,11 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">ÍNDICE DE COBERTURA EM CONSULTA MÉDICA				</t>
+          <t>ÍNDICE DE COBERTURA EM CONSULTA MÉDICA</t>
         </is>
       </c>
       <c r="E49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -4919,7 +4915,7 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>1.47</v>
+        <v>1.86</v>
       </c>
       <c r="H49" t="b">
         <v>0</v>
@@ -4928,30 +4924,32 @@
         <v>45657</v>
       </c>
       <c r="J49" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K49" t="b">
         <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M49" t="b">
         <v>0</v>
       </c>
       <c r="N49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O49" t="b">
         <v>0</v>
       </c>
-      <c r="P49" t="inlineStr"/>
+      <c r="P49" t="n">
+        <v>3</v>
+      </c>
       <c r="Q49" t="b">
         <v>0</v>
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t xml:space="preserve">SISTEMA DE CADASTRO ÚNICO (CADU) E SISTEMA DE AUTORIZAÇÃO E FATURAMENTO ELETRÔNICO (SAFE) DO IPSEMG				</t>
+          <t>SISTEMA DE CADASTRO DOS BENEFICIÁRIOS (SICAD) E SISTEMA DE AUTORIZAÇÃO E FATURAMENTO ELETRÔNICO (SAFE) DO IPSEMG</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
@@ -4966,7 +4964,7 @@
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t xml:space="preserve">[TOTAL DE CONSULTAS MÉDICAS (ELETIVAS, DE ATENÇÃO PRIMÁRIA, DE URGÊNCIA E DE PRONTO SOCORRO) REALIZADAS / TOTAL DE BENEFICIÁRIOS ATIVOS NO SISTEMA DE CADASTRO ÚNICO (CADU) DO IPSEMG]				</t>
+          <t>[TOTAL ANUAL DE CONSULTAS MÉDICAS (ELETIVAS, DE URGÊNCIA E DE PRONTO SOCORRO) REALIZADAS / MÉDIA ANUAL DO NÚMERO MENSAL DE BENEFICIÁRIOS ATIVOS NO SISTEMA DE CADASTRO DOS BENEFICIÁRIOS (SICAD)]</t>
         </is>
       </c>
       <c r="V49" t="inlineStr"/>
@@ -4975,7 +4973,7 @@
         <v>45924.50972222222</v>
       </c>
       <c r="Y49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
@@ -8834,7 +8832,7 @@
       <c r="V91" t="inlineStr"/>
       <c r="W91" t="inlineStr"/>
       <c r="X91" s="2" t="n">
-        <v>45904.44305555556</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y91" t="b">
         <v>0</v>
@@ -9687,7 +9685,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM CAFEICULTURA</t>
+          <t>CLIENTES ASSISTIDOS</t>
         </is>
       </c>
       <c r="E101" t="b">
@@ -9695,38 +9693,38 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Nº de Atendimentos Realizados</t>
+          <t>ASSISTÊNCIAS PRESTADAS</t>
         </is>
       </c>
       <c r="G101" t="n">
-        <v>110000</v>
+        <v>40000</v>
       </c>
       <c r="H101" t="b">
         <v>0</v>
       </c>
       <c r="I101" s="2" t="n">
-        <v>44926</v>
+        <v>44917</v>
       </c>
       <c r="J101" t="n">
-        <v>110000</v>
+        <v>40000</v>
       </c>
       <c r="K101" t="b">
         <v>0</v>
       </c>
       <c r="L101" t="n">
-        <v>110000</v>
+        <v>40000</v>
       </c>
       <c r="M101" t="b">
         <v>0</v>
       </c>
       <c r="N101" t="n">
-        <v>110000</v>
+        <v>40000</v>
       </c>
       <c r="O101" t="b">
         <v>0</v>
       </c>
       <c r="P101" t="n">
-        <v>110000</v>
+        <v>40000</v>
       </c>
       <c r="Q101" t="b">
         <v>0</v>
@@ -9748,7 +9746,7 @@
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>NÃO SE APLICA. VALOR ABSOLUTO.</t>
+          <t>NÃO SE APLICA. VALOR ABSOLUTO</t>
         </is>
       </c>
       <c r="V101" t="inlineStr"/>
@@ -9779,7 +9777,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM BOVINOCULTURA</t>
+          <t>ATENDIMENTOS REALIZADOS EM CAFEICULTURA</t>
         </is>
       </c>
       <c r="E102" t="b">
@@ -9791,7 +9789,7 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>220000</v>
+        <v>110000</v>
       </c>
       <c r="H102" t="b">
         <v>0</v>
@@ -9800,25 +9798,25 @@
         <v>44926</v>
       </c>
       <c r="J102" t="n">
-        <v>220000</v>
+        <v>110000</v>
       </c>
       <c r="K102" t="b">
         <v>0</v>
       </c>
       <c r="L102" t="n">
-        <v>220000</v>
+        <v>110000</v>
       </c>
       <c r="M102" t="b">
         <v>0</v>
       </c>
       <c r="N102" t="n">
-        <v>220000</v>
+        <v>110000</v>
       </c>
       <c r="O102" t="b">
         <v>0</v>
       </c>
       <c r="P102" t="n">
-        <v>220000</v>
+        <v>110000</v>
       </c>
       <c r="Q102" t="b">
         <v>0</v>
@@ -9871,7 +9869,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM COMERCIALIZAÇÃO E GESTÃO</t>
+          <t>ATENDIMENTOS REALIZADOS EM BOVINOCULTURA</t>
         </is>
       </c>
       <c r="E103" t="b">
@@ -9883,7 +9881,7 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>300000</v>
+        <v>220000</v>
       </c>
       <c r="H103" t="b">
         <v>0</v>
@@ -9892,25 +9890,25 @@
         <v>44926</v>
       </c>
       <c r="J103" t="n">
-        <v>300000</v>
+        <v>220000</v>
       </c>
       <c r="K103" t="b">
         <v>0</v>
       </c>
       <c r="L103" t="n">
-        <v>300000</v>
+        <v>220000</v>
       </c>
       <c r="M103" t="b">
         <v>0</v>
       </c>
       <c r="N103" t="n">
-        <v>300000</v>
+        <v>220000</v>
       </c>
       <c r="O103" t="b">
         <v>0</v>
       </c>
       <c r="P103" t="n">
-        <v>300000</v>
+        <v>220000</v>
       </c>
       <c r="Q103" t="b">
         <v>0</v>
@@ -9963,7 +9961,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM CRIAÇÕES</t>
+          <t>ATENDIMENTOS REALIZADOS EM COMERCIALIZAÇÃO E GESTÃO</t>
         </is>
       </c>
       <c r="E104" t="b">
@@ -9975,7 +9973,7 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>110000</v>
+        <v>300000</v>
       </c>
       <c r="H104" t="b">
         <v>0</v>
@@ -9984,25 +9982,25 @@
         <v>44926</v>
       </c>
       <c r="J104" t="n">
-        <v>110000</v>
+        <v>300000</v>
       </c>
       <c r="K104" t="b">
         <v>0</v>
       </c>
       <c r="L104" t="n">
-        <v>110000</v>
+        <v>300000</v>
       </c>
       <c r="M104" t="b">
         <v>0</v>
       </c>
       <c r="N104" t="n">
-        <v>110000</v>
+        <v>300000</v>
       </c>
       <c r="O104" t="b">
         <v>0</v>
       </c>
       <c r="P104" t="n">
-        <v>110000</v>
+        <v>300000</v>
       </c>
       <c r="Q104" t="b">
         <v>0</v>
@@ -10055,7 +10053,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM CULTURAS</t>
+          <t>ATENDIMENTOS REALIZADOS EM CRIAÇÕES</t>
         </is>
       </c>
       <c r="E105" t="b">
@@ -10067,7 +10065,7 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>170000</v>
+        <v>110000</v>
       </c>
       <c r="H105" t="b">
         <v>0</v>
@@ -10076,25 +10074,25 @@
         <v>44926</v>
       </c>
       <c r="J105" t="n">
-        <v>170000</v>
+        <v>110000</v>
       </c>
       <c r="K105" t="b">
         <v>0</v>
       </c>
       <c r="L105" t="n">
-        <v>170000</v>
+        <v>110000</v>
       </c>
       <c r="M105" t="b">
         <v>0</v>
       </c>
       <c r="N105" t="n">
-        <v>170000</v>
+        <v>110000</v>
       </c>
       <c r="O105" t="b">
         <v>0</v>
       </c>
       <c r="P105" t="n">
-        <v>170000</v>
+        <v>110000</v>
       </c>
       <c r="Q105" t="b">
         <v>0</v>
@@ -10147,7 +10145,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM HORTALIÇAS E FRUTAS</t>
+          <t>ATENDIMENTOS REALIZADOS EM CULTURAS</t>
         </is>
       </c>
       <c r="E106" t="b">
@@ -10159,7 +10157,7 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>300000</v>
+        <v>170000</v>
       </c>
       <c r="H106" t="b">
         <v>0</v>
@@ -10168,25 +10166,25 @@
         <v>44926</v>
       </c>
       <c r="J106" t="n">
-        <v>300000</v>
+        <v>170000</v>
       </c>
       <c r="K106" t="b">
         <v>0</v>
       </c>
       <c r="L106" t="n">
-        <v>300000</v>
+        <v>170000</v>
       </c>
       <c r="M106" t="b">
         <v>0</v>
       </c>
       <c r="N106" t="n">
-        <v>300000</v>
+        <v>170000</v>
       </c>
       <c r="O106" t="b">
         <v>0</v>
       </c>
       <c r="P106" t="n">
-        <v>300000</v>
+        <v>170000</v>
       </c>
       <c r="Q106" t="b">
         <v>0</v>
@@ -10239,7 +10237,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM INCLUSÃO PRODUTIVA</t>
+          <t>ATENDIMENTOS REALIZADOS EM HORTALIÇAS E FRUTAS</t>
         </is>
       </c>
       <c r="E107" t="b">
@@ -10251,7 +10249,7 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>480000</v>
+        <v>300000</v>
       </c>
       <c r="H107" t="b">
         <v>0</v>
@@ -10260,25 +10258,25 @@
         <v>44926</v>
       </c>
       <c r="J107" t="n">
-        <v>480000</v>
+        <v>300000</v>
       </c>
       <c r="K107" t="b">
         <v>0</v>
       </c>
       <c r="L107" t="n">
-        <v>480000</v>
+        <v>300000</v>
       </c>
       <c r="M107" t="b">
         <v>0</v>
       </c>
       <c r="N107" t="n">
-        <v>480000</v>
+        <v>300000</v>
       </c>
       <c r="O107" t="b">
         <v>0</v>
       </c>
       <c r="P107" t="n">
-        <v>480000</v>
+        <v>300000</v>
       </c>
       <c r="Q107" t="b">
         <v>0</v>
@@ -10331,7 +10329,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM SEGURANÇA HÍDRICA E SUSTENTABILIDADE AMBIENTAL</t>
+          <t>ATENDIMENTOS REALIZADOS EM INCLUSÃO PRODUTIVA</t>
         </is>
       </c>
       <c r="E108" t="b">
@@ -10343,7 +10341,7 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>240000</v>
+        <v>480000</v>
       </c>
       <c r="H108" t="b">
         <v>0</v>
@@ -10352,25 +10350,25 @@
         <v>44926</v>
       </c>
       <c r="J108" t="n">
-        <v>240000</v>
+        <v>480000</v>
       </c>
       <c r="K108" t="b">
         <v>0</v>
       </c>
       <c r="L108" t="n">
-        <v>240000</v>
+        <v>480000</v>
       </c>
       <c r="M108" t="b">
         <v>0</v>
       </c>
       <c r="N108" t="n">
-        <v>240000</v>
+        <v>480000</v>
       </c>
       <c r="O108" t="b">
         <v>0</v>
       </c>
       <c r="P108" t="n">
-        <v>240000</v>
+        <v>480000</v>
       </c>
       <c r="Q108" t="b">
         <v>0</v>
@@ -10423,7 +10421,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>ATENDIMENTOS REALIZADOS EM AGROECOLOGIA</t>
+          <t>ATENDIMENTOS REALIZADOS EM SEGURANÇA HÍDRICA E SUSTENTABILIDADE AMBIENTAL</t>
         </is>
       </c>
       <c r="E109" t="b">
@@ -10435,7 +10433,7 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>70000</v>
+        <v>240000</v>
       </c>
       <c r="H109" t="b">
         <v>0</v>
@@ -10444,25 +10442,25 @@
         <v>44926</v>
       </c>
       <c r="J109" t="n">
-        <v>70000</v>
+        <v>240000</v>
       </c>
       <c r="K109" t="b">
         <v>0</v>
       </c>
       <c r="L109" t="n">
-        <v>70000</v>
+        <v>240000</v>
       </c>
       <c r="M109" t="b">
         <v>0</v>
       </c>
       <c r="N109" t="n">
-        <v>70000</v>
+        <v>240000</v>
       </c>
       <c r="O109" t="b">
         <v>0</v>
       </c>
       <c r="P109" t="n">
-        <v>70000</v>
+        <v>240000</v>
       </c>
       <c r="Q109" t="b">
         <v>0</v>
@@ -10515,7 +10513,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>CLIENTES ASSISTIDOS</t>
+          <t>ATENDIMENTOS REALIZADOS EM AGROECOLOGIA</t>
         </is>
       </c>
       <c r="E110" t="b">
@@ -10523,38 +10521,38 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>ASSISTÊNCIAS PRESTADAS</t>
+          <t>Nº de Atendimentos Realizados</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="H110" t="b">
         <v>0</v>
       </c>
       <c r="I110" s="2" t="n">
-        <v>44917</v>
+        <v>44926</v>
       </c>
       <c r="J110" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="K110" t="b">
         <v>0</v>
       </c>
       <c r="L110" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="M110" t="b">
         <v>0</v>
       </c>
       <c r="N110" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="O110" t="b">
         <v>0</v>
       </c>
       <c r="P110" t="n">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="Q110" t="b">
         <v>0</v>
@@ -10576,7 +10574,7 @@
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>NÃO SE APLICA. VALOR ABSOLUTO</t>
+          <t>NÃO SE APLICA. VALOR ABSOLUTO.</t>
         </is>
       </c>
       <c r="V110" t="inlineStr"/>
@@ -10607,11 +10605,11 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>DISCENTES FORMADOS E CAPACITADOS</t>
+          <t>PESQUISA/ATIVIDADE REALIZADA</t>
         </is>
       </c>
       <c r="E111" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -10624,32 +10622,30 @@
       </c>
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="n">
-        <v>1955</v>
+        <v>5</v>
       </c>
       <c r="K111" t="b">
         <v>0</v>
       </c>
       <c r="L111" t="n">
-        <v>1895</v>
+        <v>5</v>
       </c>
       <c r="M111" t="b">
         <v>0</v>
       </c>
       <c r="N111" t="n">
-        <v>1918</v>
+        <v>5</v>
       </c>
       <c r="O111" t="b">
         <v>0</v>
       </c>
-      <c r="P111" t="n">
-        <v>1918</v>
-      </c>
+      <c r="P111" t="inlineStr"/>
       <c r="Q111" t="b">
         <v>0</v>
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>ESCOLA DE GOVERNO PROFESSOR PAULO NEVES DE CARVALHO</t>
+          <t>FJP/ESCOLA DE GOVERNO/GERENCIA DE ENSINO E PESQUISA</t>
         </is>
       </c>
       <c r="S111" t="inlineStr">
@@ -10664,20 +10660,16 @@
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>NÚMERO DE ALUNOS/DISCENTES MATRICULADOS/ATENDIDOS NOS CURSOS DA ESCOLA DE GOVERNO - GRADUAÇÃO, ESPECIALIZAÇÃO, MESTRADO, FORMAÇÃO EXECUTIVA E CONTINUADA - QUE EFETIVAMENTE CONCLUEM OS CURSOS.</t>
+          <t>SOMA DO NÚMERO DE PESQUISAS, ESTUDOS E ATIVIDADES REALIZADAS NO AMBITO DOS GRUPOS DE PESQUISA.</t>
         </is>
       </c>
       <c r="V111" t="inlineStr"/>
-      <c r="W111" t="inlineStr">
-        <is>
-          <t>QUANTO À INEXISTÊNCIA DOS ÍNDICES DE REFERÊNCIA, OS MESMOS ESTÃO EM APURAÇÃO. TRATAM-SE DE INDICADORES NOVOS E NÃO CONSEGUIMOS APURAR O "PARA TRÁS" A TEMPO.</t>
-        </is>
-      </c>
+      <c r="W111" t="inlineStr"/>
       <c r="X111" s="2" t="n">
         <v>45923.45763888889</v>
       </c>
       <c r="Y111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z111" t="inlineStr">
         <is>
@@ -10699,11 +10691,11 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>PESQUISA/ATIVIDADE REALIZADA</t>
+          <t>DISCENTES FORMADOS E CAPACITADOS</t>
         </is>
       </c>
       <c r="E112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -10716,30 +10708,32 @@
       </c>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="n">
-        <v>5</v>
+        <v>1955</v>
       </c>
       <c r="K112" t="b">
         <v>0</v>
       </c>
       <c r="L112" t="n">
-        <v>5</v>
+        <v>1895</v>
       </c>
       <c r="M112" t="b">
         <v>0</v>
       </c>
       <c r="N112" t="n">
-        <v>5</v>
+        <v>1918</v>
       </c>
       <c r="O112" t="b">
         <v>0</v>
       </c>
-      <c r="P112" t="inlineStr"/>
+      <c r="P112" t="n">
+        <v>1918</v>
+      </c>
       <c r="Q112" t="b">
         <v>0</v>
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>FJP/ESCOLA DE GOVERNO/GERENCIA DE ENSINO E PESQUISA</t>
+          <t>ESCOLA DE GOVERNO PROFESSOR PAULO NEVES DE CARVALHO</t>
         </is>
       </c>
       <c r="S112" t="inlineStr">
@@ -10754,16 +10748,20 @@
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>SOMA DO NÚMERO DE PESQUISAS, ESTUDOS E ATIVIDADES REALIZADAS NO AMBITO DOS GRUPOS DE PESQUISA.</t>
+          <t>NÚMERO DE ALUNOS/DISCENTES MATRICULADOS/ATENDIDOS NOS CURSOS DA ESCOLA DE GOVERNO - GRADUAÇÃO, ESPECIALIZAÇÃO, MESTRADO, FORMAÇÃO EXECUTIVA E CONTINUADA - QUE EFETIVAMENTE CONCLUEM OS CURSOS.</t>
         </is>
       </c>
       <c r="V112" t="inlineStr"/>
-      <c r="W112" t="inlineStr"/>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>QUANTO À INEXISTÊNCIA DOS ÍNDICES DE REFERÊNCIA, OS MESMOS ESTÃO EM APURAÇÃO. TRATAM-SE DE INDICADORES NOVOS E NÃO CONSEGUIMOS APURAR O "PARA TRÁS" A TEMPO.</t>
+        </is>
+      </c>
       <c r="X112" s="2" t="n">
         <v>45923.45763888889</v>
       </c>
       <c r="Y112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z112" t="inlineStr">
         <is>
@@ -10877,47 +10875,53 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>TAXA DE EVASÃO</t>
+          <t>DESEMPENHO DOS DISCENTES DA GRADUAÇÃO NO ENADE - EXAME NACIONAL DE DESEMPENHO DOS ESTUDANTES</t>
         </is>
       </c>
       <c r="E114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr"/>
+          <t>Nota</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>5</v>
+      </c>
       <c r="H114" t="b">
-        <v>1</v>
-      </c>
-      <c r="I114" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I114" s="2" t="n">
+        <v>44926</v>
+      </c>
       <c r="J114" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="K114" t="b">
         <v>0</v>
       </c>
       <c r="L114" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="M114" t="b">
         <v>0</v>
       </c>
       <c r="N114" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="O114" t="b">
         <v>0</v>
       </c>
-      <c r="P114" t="inlineStr"/>
+      <c r="P114" t="n">
+        <v>5</v>
+      </c>
       <c r="Q114" t="b">
         <v>0</v>
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>FUNDAÇÃO JOÃO PINHEIRO - ESCOLA DE GOVERNO</t>
+          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
         </is>
       </c>
       <c r="S114" t="inlineStr">
@@ -10927,12 +10931,13 @@
       </c>
       <c r="T114" t="inlineStr">
         <is>
-          <t>Estadual</t>
-        </is>
-      </c>
-      <c r="U114">
-        <f> [(PESSOA CAPACITADA PLANEJADO - PESSOA CAPACITADA EXECUTADO) / PESSOA CAPACITADA PLANEJADO] X 100</f>
-        <v/>
+          <t>Nacional</t>
+        </is>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>O ENADE, OU EXAME NACIONAL DE DESEMPENHO DOS ESTUDANTES, É UMA AVALIAÇÃO DO MINISTÉRIO DA EDUCAÇÃO (MEC) QUE VISA MEDIR O DESEMPENHO DOS ALUNOS CONCLUINTES DE CURSOS DE GRADUAÇÃO EM RELAÇÃO AOS CONTEÚDOS PROGRAMÁTICOS PREVISTOS NAS DIRETRIZES CURRICULARES, BEM COMO O DESENVOLVIMENTO DE COMPETÊNCIAS E HABILIDADES. O EXAME SERVE COMO UM INDICADOR DA QUALIDADE DO ENSINO SUPERIOR NO BRASIL, AUXILIANDO O MEC NA FORMULAÇÃO DE POLÍTICAS PÚBLICAS NA ÁREA DA EDUCAÇÃO E AVALIANDO A QUALIDADE DAS INSTITUIÇÕES DE ENSINO. FÓRMULA DE CÁLCULO COMPLETA DISPONÍVEL EM: HTTPS://WWW.GOV.BR/INEP/PT-BR/AREAS-DE-ATUACAO/AVALIACAO-E-EXAMES-EDUCACIONAIS/ENADE</t>
+        </is>
       </c>
       <c r="V114" t="inlineStr"/>
       <c r="W114" t="inlineStr"/>
@@ -10940,11 +10945,11 @@
         <v>45923.45763888889</v>
       </c>
       <c r="Y114" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z114" t="inlineStr">
         <is>
-          <t>MENOR</t>
+          <t>MAIOR</t>
         </is>
       </c>
     </row>
@@ -11054,53 +11059,47 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>DESEMPENHO DOS DISCENTES DA GRADUAÇÃO NO ENADE - EXAME NACIONAL DE DESEMPENHO DOS ESTUDANTES</t>
+          <t>TAXA DE EVASÃO</t>
         </is>
       </c>
       <c r="E116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Nota</t>
-        </is>
-      </c>
-      <c r="G116" t="n">
-        <v>5</v>
-      </c>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
       <c r="H116" t="b">
-        <v>0</v>
-      </c>
-      <c r="I116" s="2" t="n">
-        <v>44926</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I116" t="inlineStr"/>
       <c r="J116" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="K116" t="b">
         <v>0</v>
       </c>
       <c r="L116" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="M116" t="b">
         <v>0</v>
       </c>
       <c r="N116" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="O116" t="b">
         <v>0</v>
       </c>
-      <c r="P116" t="n">
-        <v>5</v>
-      </c>
+      <c r="P116" t="inlineStr"/>
       <c r="Q116" t="b">
         <v>0</v>
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
+          <t>FUNDAÇÃO JOÃO PINHEIRO - ESCOLA DE GOVERNO</t>
         </is>
       </c>
       <c r="S116" t="inlineStr">
@@ -11110,13 +11109,12 @@
       </c>
       <c r="T116" t="inlineStr">
         <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>O ENADE, OU EXAME NACIONAL DE DESEMPENHO DOS ESTUDANTES, É UMA AVALIAÇÃO DO MINISTÉRIO DA EDUCAÇÃO (MEC) QUE VISA MEDIR O DESEMPENHO DOS ALUNOS CONCLUINTES DE CURSOS DE GRADUAÇÃO EM RELAÇÃO AOS CONTEÚDOS PROGRAMÁTICOS PREVISTOS NAS DIRETRIZES CURRICULARES, BEM COMO O DESENVOLVIMENTO DE COMPETÊNCIAS E HABILIDADES. O EXAME SERVE COMO UM INDICADOR DA QUALIDADE DO ENSINO SUPERIOR NO BRASIL, AUXILIANDO O MEC NA FORMULAÇÃO DE POLÍTICAS PÚBLICAS NA ÁREA DA EDUCAÇÃO E AVALIANDO A QUALIDADE DAS INSTITUIÇÕES DE ENSINO. FÓRMULA DE CÁLCULO COMPLETA DISPONÍVEL EM: HTTPS://WWW.GOV.BR/INEP/PT-BR/AREAS-DE-ATUACAO/AVALIACAO-E-EXAMES-EDUCACIONAIS/ENADE</t>
-        </is>
+          <t>Estadual</t>
+        </is>
+      </c>
+      <c r="U116">
+        <f> [(PESSOA CAPACITADA PLANEJADO - PESSOA CAPACITADA EXECUTADO) / PESSOA CAPACITADA PLANEJADO] X 100</f>
+        <v/>
       </c>
       <c r="V116" t="inlineStr"/>
       <c r="W116" t="inlineStr"/>
@@ -11124,11 +11122,11 @@
         <v>45923.45763888889</v>
       </c>
       <c r="Y116" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z116" t="inlineStr">
         <is>
-          <t>MAIOR</t>
+          <t>MENOR</t>
         </is>
       </c>
     </row>
@@ -11453,7 +11451,7 @@
         <v>0</v>
       </c>
       <c r="P120" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q120" t="b">
         <v>0</v>
@@ -11485,7 +11483,7 @@
         </is>
       </c>
       <c r="X120" s="2" t="n">
-        <v>45917.52291666667</v>
+        <v>45925.46458333333</v>
       </c>
       <c r="Y120" t="b">
         <v>0</v>
@@ -11757,7 +11755,7 @@
       <c r="V123" t="inlineStr"/>
       <c r="W123" t="inlineStr"/>
       <c r="X123" s="2" t="n">
-        <v>45888.46736111111</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y123" t="b">
         <v>0</v>
@@ -11849,7 +11847,7 @@
       <c r="V124" t="inlineStr"/>
       <c r="W124" t="inlineStr"/>
       <c r="X124" s="2" t="n">
-        <v>45888.61805555555</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y124" t="b">
         <v>0</v>
@@ -11874,7 +11872,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>NÚMERO DE ATIVIDADES CULTURAIS DA ORQUESTRA FILARMÔNICA, ORQUESTRA SINFÔNICA, CORAL LÍRICO DA CIA DE DANÇA, DO CINE HUMBERTO MAURO, ARTES VISUAIS</t>
+          <t>PÚBLICO DO CIRCUITO LIBERDADE</t>
         </is>
       </c>
       <c r="E125" t="b">
@@ -11882,45 +11880,45 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Atividade</t>
+          <t>visitante</t>
         </is>
       </c>
       <c r="G125" t="n">
-        <v>6490</v>
+        <v>5154019</v>
       </c>
       <c r="H125" t="b">
         <v>0</v>
       </c>
       <c r="I125" s="2" t="n">
-        <v>45657</v>
+        <v>45291</v>
       </c>
       <c r="J125" t="n">
-        <v>4674</v>
+        <v>1725441</v>
       </c>
       <c r="K125" t="b">
         <v>0</v>
       </c>
       <c r="L125" t="n">
-        <v>4725</v>
+        <v>2711407</v>
       </c>
       <c r="M125" t="b">
         <v>0</v>
       </c>
       <c r="N125" t="n">
-        <v>4776</v>
+        <v>3253688</v>
       </c>
       <c r="O125" t="b">
         <v>0</v>
       </c>
       <c r="P125" t="n">
-        <v>4827</v>
+        <v>3579056</v>
       </c>
       <c r="Q125" t="b">
         <v>0</v>
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>FUNDAÇÃO CLÓVIS SALGADO E SECULT (COMISSÃO SUPERVISORA DO CONTRATO DE GESTÃO DA ORQUESTRA FILARMÔNICA)</t>
+          <t>FUNDAÇÃO CLÓVIS SALGADO - FCS</t>
         </is>
       </c>
       <c r="S125" t="inlineStr">
@@ -11930,21 +11928,21 @@
       </c>
       <c r="T125" t="inlineStr">
         <is>
-          <t>Estadual</t>
+          <t>Municipal</t>
         </is>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>SOMATÓRIO DAS ATIVIDADES DESENVOLVIDAS PELA ORQUESTRA FILARMÔNICA, ORQUESTRA SINFÔNICA, CORAL LÍRICO, CIA DE DANÇA, CINE HUMBERTO MAURO, ARTES VISUAIS</t>
+          <t>SOMA DO NÚMERO DE VISITANTES PRESENCIAIS E DO NÚMERO DE PARTICIPANTES DAS AÇÕES REALIZADAS NO TERRITÓRIO DEFINIDO PELO § 1º, ART. 2º DECRETO Nº 48.074/2020, DESDE QUE VINCULADAS AOS EQUIPAMENTOS CULTURAIS DO CIRCUITO LIBERDADE.</t>
         </is>
       </c>
       <c r="V125" t="inlineStr"/>
       <c r="W125" t="inlineStr"/>
       <c r="X125" s="2" t="n">
-        <v>45888.47430555556</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y125" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z125" t="inlineStr">
         <is>
@@ -11966,7 +11964,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>PÚBLICO DO CIRCUITO LIBERDADE</t>
+          <t>NÚMERO DE ATIVIDADES CULTURAIS DA ORQUESTRA FILARMÔNICA, ORQUESTRA SINFÔNICA, CORAL LÍRICO DA CIA DE DANÇA, DO CINE HUMBERTO MAURO, ARTES VISUAIS</t>
         </is>
       </c>
       <c r="E126" t="b">
@@ -11974,45 +11972,45 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>visitante</t>
+          <t>Atividade</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>5154019</v>
+        <v>6490</v>
       </c>
       <c r="H126" t="b">
         <v>0</v>
       </c>
       <c r="I126" s="2" t="n">
-        <v>45291</v>
+        <v>45657</v>
       </c>
       <c r="J126" t="n">
-        <v>1725441</v>
+        <v>4674</v>
       </c>
       <c r="K126" t="b">
         <v>0</v>
       </c>
       <c r="L126" t="n">
-        <v>2711407</v>
+        <v>4725</v>
       </c>
       <c r="M126" t="b">
         <v>0</v>
       </c>
       <c r="N126" t="n">
-        <v>3253688</v>
+        <v>4776</v>
       </c>
       <c r="O126" t="b">
         <v>0</v>
       </c>
       <c r="P126" t="n">
-        <v>3579056</v>
+        <v>4827</v>
       </c>
       <c r="Q126" t="b">
         <v>0</v>
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>FUNDAÇÃO CLÓVIS SALGADO - FCS</t>
+          <t>FUNDAÇÃO CLÓVIS SALGADO E SECULT (COMISSÃO SUPERVISORA DO CONTRATO DE GESTÃO DA ORQUESTRA FILARMÔNICA)</t>
         </is>
       </c>
       <c r="S126" t="inlineStr">
@@ -12022,21 +12020,21 @@
       </c>
       <c r="T126" t="inlineStr">
         <is>
-          <t>Municipal</t>
+          <t>Estadual</t>
         </is>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>SOMA DO NÚMERO DE VISITANTES PRESENCIAIS E DO NÚMERO DE PARTICIPANTES DAS AÇÕES REALIZADAS NO TERRITÓRIO DEFINIDO PELO § 1º, ART. 2º DECRETO Nº 48.074/2020, DESDE QUE VINCULADAS AOS EQUIPAMENTOS CULTURAIS DO CIRCUITO LIBERDADE.</t>
+          <t>SOMATÓRIO DAS ATIVIDADES DESENVOLVIDAS PELA ORQUESTRA FILARMÔNICA, ORQUESTRA SINFÔNICA, CORAL LÍRICO, CIA DE DANÇA, CINE HUMBERTO MAURO, ARTES VISUAIS</t>
         </is>
       </c>
       <c r="V126" t="inlineStr"/>
       <c r="W126" t="inlineStr"/>
       <c r="X126" s="2" t="n">
-        <v>45888.57569444444</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y126" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z126" t="inlineStr">
         <is>
@@ -12125,7 +12123,7 @@
       <c r="V127" t="inlineStr"/>
       <c r="W127" t="inlineStr"/>
       <c r="X127" s="2" t="n">
-        <v>45888.47638888889</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y127" t="b">
         <v>0</v>
@@ -12585,7 +12583,7 @@
       <c r="V132" t="inlineStr"/>
       <c r="W132" t="inlineStr"/>
       <c r="X132" s="2" t="n">
-        <v>45882.40902777778</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y132" t="b">
         <v>0</v>
@@ -14331,7 +14329,7 @@
       <c r="V151" t="inlineStr"/>
       <c r="W151" t="inlineStr"/>
       <c r="X151" s="2" t="n">
-        <v>45916.44027777778</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y151" t="b">
         <v>0</v>
@@ -14423,7 +14421,7 @@
       <c r="V152" t="inlineStr"/>
       <c r="W152" t="inlineStr"/>
       <c r="X152" s="2" t="n">
-        <v>45916.44305555556</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y152" t="b">
         <v>0</v>
@@ -14515,7 +14513,7 @@
       <c r="V153" t="inlineStr"/>
       <c r="W153" t="inlineStr"/>
       <c r="X153" s="2" t="n">
-        <v>45916.44236111111</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y153" t="b">
         <v>0</v>
@@ -14607,7 +14605,7 @@
       <c r="V154" t="inlineStr"/>
       <c r="W154" t="inlineStr"/>
       <c r="X154" s="2" t="n">
-        <v>45916.44375</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y154" t="b">
         <v>0</v>
@@ -14699,7 +14697,7 @@
       <c r="V155" t="inlineStr"/>
       <c r="W155" t="inlineStr"/>
       <c r="X155" s="2" t="n">
-        <v>45916.44166666667</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y155" t="b">
         <v>0</v>
@@ -14791,7 +14789,7 @@
       <c r="V156" t="inlineStr"/>
       <c r="W156" t="inlineStr"/>
       <c r="X156" s="2" t="n">
-        <v>45916.44097222222</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y156" t="b">
         <v>0</v>
@@ -17815,7 +17813,7 @@
       <c r="V189" t="inlineStr"/>
       <c r="W189" t="inlineStr"/>
       <c r="X189" s="2" t="n">
-        <v>45915.49861111111</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y189" t="b">
         <v>0</v>
@@ -17907,7 +17905,7 @@
       <c r="V190" t="inlineStr"/>
       <c r="W190" t="inlineStr"/>
       <c r="X190" s="2" t="n">
-        <v>45915.49861111111</v>
+        <v>45924.82708333333</v>
       </c>
       <c r="Y190" t="b">
         <v>0</v>
@@ -17932,7 +17930,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL DO 5° ANO DO ENSINO FUNDAMENTAL EM LÍNGUA PORTUGUESA (PROEB)</t>
+          <t>IDEB ANOS INICIAIS DO ENSINO FUNDAMENTAL</t>
         </is>
       </c>
       <c r="E191" t="b">
@@ -17944,7 +17942,7 @@
         </is>
       </c>
       <c r="G191" t="n">
-        <v>217.8</v>
+        <v>6.3</v>
       </c>
       <c r="H191" t="b">
         <v>0</v>
@@ -17953,37 +17951,37 @@
         <v>45537</v>
       </c>
       <c r="J191" t="n">
-        <v>225.87</v>
+        <v>0</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
       </c>
       <c r="L191" t="n">
-        <v>228.6</v>
+        <v>7</v>
       </c>
       <c r="M191" t="b">
         <v>0</v>
       </c>
       <c r="N191" t="n">
-        <v>231.41</v>
+        <v>0</v>
       </c>
       <c r="O191" t="b">
         <v>0</v>
       </c>
       <c r="P191" t="n">
-        <v>235</v>
+        <v>7.2</v>
       </c>
       <c r="Q191" t="b">
         <v>0</v>
       </c>
       <c r="R191" t="inlineStr">
         <is>
-          <t>SISTEMA MINEIRO DE AVALIAÇÃO E EQUIDADE DA EDUCAÇÃO PÚBLICA - SIMAVE</t>
+          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
         </is>
       </c>
       <c r="S191" t="inlineStr">
         <is>
-          <t>Anual</t>
+          <t>Bianual</t>
         </is>
       </c>
       <c r="T191" t="inlineStr">
@@ -17993,7 +17991,7 @@
       </c>
       <c r="U191" t="inlineStr">
         <is>
-          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM LÍNGUA PORTUGUESA.</t>
+          <t>DESEMPENHO NAS AVALIAÇÕES DO SAEB X INDICADOR DE RENDIMENTO</t>
         </is>
       </c>
       <c r="V191" t="inlineStr"/>
@@ -18024,7 +18022,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL DO 9° ANO DO ENSINO FUNDAMENTAL EM LÍNGUA PORTUGUESA (PROEB)</t>
+          <t>IDEB ENSINO MÉDIO</t>
         </is>
       </c>
       <c r="E192" t="b">
@@ -18036,7 +18034,7 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>252.7</v>
+        <v>4</v>
       </c>
       <c r="H192" t="b">
         <v>0</v>
@@ -18045,37 +18043,37 @@
         <v>45537</v>
       </c>
       <c r="J192" t="n">
-        <v>260.17</v>
+        <v>0</v>
       </c>
       <c r="K192" t="b">
         <v>0</v>
       </c>
       <c r="L192" t="n">
-        <v>266.84</v>
+        <v>4.7</v>
       </c>
       <c r="M192" t="b">
         <v>0</v>
       </c>
       <c r="N192" t="n">
-        <v>273.68</v>
+        <v>0</v>
       </c>
       <c r="O192" t="b">
         <v>0</v>
       </c>
       <c r="P192" t="n">
-        <v>275</v>
+        <v>4.8</v>
       </c>
       <c r="Q192" t="b">
         <v>0</v>
       </c>
       <c r="R192" t="inlineStr">
         <is>
-          <t>SISTEMA MINEIRO DE AVALIAÇÃO E EQUIDADE DA EDUCAÇÃO PÚBLICA - SIMAVE</t>
+          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
         </is>
       </c>
       <c r="S192" t="inlineStr">
         <is>
-          <t>Anual</t>
+          <t>Bianual</t>
         </is>
       </c>
       <c r="T192" t="inlineStr">
@@ -18085,7 +18083,7 @@
       </c>
       <c r="U192" t="inlineStr">
         <is>
-          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM LÍNGUA PORTUGUESA.</t>
+          <t>DESEMPENHO NAS AVALIAÇÕES DO SAEB X INDICADOR DE RENDIMENTO</t>
         </is>
       </c>
       <c r="V192" t="inlineStr"/>
@@ -18116,7 +18114,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL  DO 3° ANO DO ENSINO MÉDIO EM MATEMÁTICA (PROEB)</t>
+          <t>IDEB ANOS FINAIS DO ENSINO FUNDAMENTAL</t>
         </is>
       </c>
       <c r="E193" t="b">
@@ -18128,7 +18126,7 @@
         </is>
       </c>
       <c r="G193" t="n">
-        <v>269.4</v>
+        <v>4.6</v>
       </c>
       <c r="H193" t="b">
         <v>0</v>
@@ -18137,37 +18135,37 @@
         <v>45537</v>
       </c>
       <c r="J193" t="n">
-        <v>276.52</v>
+        <v>0</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
       </c>
       <c r="L193" t="n">
-        <v>282.05</v>
+        <v>6.4</v>
       </c>
       <c r="M193" t="b">
         <v>0</v>
       </c>
       <c r="N193" t="n">
-        <v>287.69</v>
+        <v>0</v>
       </c>
       <c r="O193" t="b">
         <v>0</v>
       </c>
       <c r="P193" t="n">
-        <v>293</v>
+        <v>6.6</v>
       </c>
       <c r="Q193" t="b">
         <v>0</v>
       </c>
       <c r="R193" t="inlineStr">
         <is>
-          <t>SISTEMA MINEIRO DE AVALIAÇÃO E EQUIDADE DA EDUCAÇÃO PÚBLICA - SIMAVE</t>
+          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
         </is>
       </c>
       <c r="S193" t="inlineStr">
         <is>
-          <t>Anual</t>
+          <t>Bianual</t>
         </is>
       </c>
       <c r="T193" t="inlineStr">
@@ -18177,7 +18175,7 @@
       </c>
       <c r="U193" t="inlineStr">
         <is>
-          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM MATEMÁTICA.</t>
+          <t>DESEMPENHO NAS AVALIAÇÕES DO SAEB X INDICADOR DE RENDIMENTO</t>
         </is>
       </c>
       <c r="V193" t="inlineStr"/>
@@ -18208,7 +18206,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL  DO 9° ANO DO ENSINO FUNDAMENTAL  EM MATEMÁTICA (PROEB)</t>
+          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL DO 5° ANO DO ENSINO FUNDAMENTAL EM LÍNGUA PORTUGUESA (PROEB)</t>
         </is>
       </c>
       <c r="E194" t="b">
@@ -18220,7 +18218,7 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>249.3</v>
+        <v>217.8</v>
       </c>
       <c r="H194" t="b">
         <v>0</v>
@@ -18229,25 +18227,25 @@
         <v>45537</v>
       </c>
       <c r="J194" t="n">
-        <v>267.05</v>
+        <v>225.87</v>
       </c>
       <c r="K194" t="b">
         <v>0</v>
       </c>
       <c r="L194" t="n">
-        <v>275.11</v>
+        <v>228.6</v>
       </c>
       <c r="M194" t="b">
         <v>0</v>
       </c>
       <c r="N194" t="n">
-        <v>283.41</v>
+        <v>231.41</v>
       </c>
       <c r="O194" t="b">
         <v>0</v>
       </c>
       <c r="P194" t="n">
-        <v>288</v>
+        <v>235</v>
       </c>
       <c r="Q194" t="b">
         <v>0</v>
@@ -18269,7 +18267,7 @@
       </c>
       <c r="U194" t="inlineStr">
         <is>
-          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM MATEMÁTICA.</t>
+          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM LÍNGUA PORTUGUESA.</t>
         </is>
       </c>
       <c r="V194" t="inlineStr"/>
@@ -18300,7 +18298,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>PROFICIÊNCIA MÉDIA DOS ALUNOS DO 3° ANO DO ENSINO MÉDIO EM LÍNGUA PORTUGUESA (PROEB)</t>
+          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL DO 9° ANO DO ENSINO FUNDAMENTAL EM LÍNGUA PORTUGUESA (PROEB)</t>
         </is>
       </c>
       <c r="E195" t="b">
@@ -18312,7 +18310,7 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>273.2</v>
+        <v>252.7</v>
       </c>
       <c r="H195" t="b">
         <v>0</v>
@@ -18321,25 +18319,25 @@
         <v>45537</v>
       </c>
       <c r="J195" t="n">
-        <v>281.41</v>
+        <v>260.17</v>
       </c>
       <c r="K195" t="b">
         <v>0</v>
       </c>
       <c r="L195" t="n">
-        <v>287.04</v>
+        <v>266.84</v>
       </c>
       <c r="M195" t="b">
         <v>0</v>
       </c>
       <c r="N195" t="n">
-        <v>292.78</v>
+        <v>273.68</v>
       </c>
       <c r="O195" t="b">
         <v>0</v>
       </c>
       <c r="P195" t="n">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="Q195" t="b">
         <v>0</v>
@@ -18361,7 +18359,7 @@
       </c>
       <c r="U195" t="inlineStr">
         <is>
-          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM LÍNGUA PORTUGUESA</t>
+          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM LÍNGUA PORTUGUESA.</t>
         </is>
       </c>
       <c r="V195" t="inlineStr"/>
@@ -18392,7 +18390,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL NO 5° ANO DO ENSINO FUNDAMENTAL EM MATEMÁTICA (PROEB)</t>
+          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL  DO 3° ANO DO ENSINO MÉDIO EM MATEMÁTICA (PROEB)</t>
         </is>
       </c>
       <c r="E196" t="b">
@@ -18404,7 +18402,7 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>227.2</v>
+        <v>269.4</v>
       </c>
       <c r="H196" t="b">
         <v>0</v>
@@ -18413,25 +18411,25 @@
         <v>45537</v>
       </c>
       <c r="J196" t="n">
-        <v>242.26</v>
+        <v>276.52</v>
       </c>
       <c r="K196" t="b">
         <v>0</v>
       </c>
       <c r="L196" t="n">
-        <v>250.31</v>
+        <v>282.05</v>
       </c>
       <c r="M196" t="b">
         <v>0</v>
       </c>
       <c r="N196" t="n">
-        <v>252.7</v>
+        <v>287.69</v>
       </c>
       <c r="O196" t="b">
         <v>0</v>
       </c>
       <c r="P196" t="n">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="Q196" t="b">
         <v>0</v>
@@ -18484,7 +18482,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>IDEB ANOS INICIAIS DO ENSINO FUNDAMENTAL</t>
+          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL  DO 9° ANO DO ENSINO FUNDAMENTAL  EM MATEMÁTICA (PROEB)</t>
         </is>
       </c>
       <c r="E197" t="b">
@@ -18496,7 +18494,7 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>6.3</v>
+        <v>249.3</v>
       </c>
       <c r="H197" t="b">
         <v>0</v>
@@ -18505,37 +18503,37 @@
         <v>45537</v>
       </c>
       <c r="J197" t="n">
-        <v>0</v>
+        <v>267.05</v>
       </c>
       <c r="K197" t="b">
         <v>0</v>
       </c>
       <c r="L197" t="n">
-        <v>7</v>
+        <v>275.11</v>
       </c>
       <c r="M197" t="b">
         <v>0</v>
       </c>
       <c r="N197" t="n">
-        <v>0</v>
+        <v>283.41</v>
       </c>
       <c r="O197" t="b">
         <v>0</v>
       </c>
       <c r="P197" t="n">
-        <v>7.2</v>
+        <v>288</v>
       </c>
       <c r="Q197" t="b">
         <v>0</v>
       </c>
       <c r="R197" t="inlineStr">
         <is>
-          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
+          <t>SISTEMA MINEIRO DE AVALIAÇÃO E EQUIDADE DA EDUCAÇÃO PÚBLICA - SIMAVE</t>
         </is>
       </c>
       <c r="S197" t="inlineStr">
         <is>
-          <t>Bianual</t>
+          <t>Anual</t>
         </is>
       </c>
       <c r="T197" t="inlineStr">
@@ -18545,7 +18543,7 @@
       </c>
       <c r="U197" t="inlineStr">
         <is>
-          <t>DESEMPENHO NAS AVALIAÇÕES DO SAEB X INDICADOR DE RENDIMENTO</t>
+          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM MATEMÁTICA.</t>
         </is>
       </c>
       <c r="V197" t="inlineStr"/>
@@ -18576,7 +18574,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>IDEB ENSINO MÉDIO</t>
+          <t>PROFICIÊNCIA MÉDIA DOS ALUNOS DO 3° ANO DO ENSINO MÉDIO EM LÍNGUA PORTUGUESA (PROEB)</t>
         </is>
       </c>
       <c r="E198" t="b">
@@ -18588,7 +18586,7 @@
         </is>
       </c>
       <c r="G198" t="n">
-        <v>4</v>
+        <v>273.2</v>
       </c>
       <c r="H198" t="b">
         <v>0</v>
@@ -18597,37 +18595,37 @@
         <v>45537</v>
       </c>
       <c r="J198" t="n">
-        <v>0</v>
+        <v>281.41</v>
       </c>
       <c r="K198" t="b">
         <v>0</v>
       </c>
       <c r="L198" t="n">
-        <v>4.7</v>
+        <v>287.04</v>
       </c>
       <c r="M198" t="b">
         <v>0</v>
       </c>
       <c r="N198" t="n">
-        <v>0</v>
+        <v>292.78</v>
       </c>
       <c r="O198" t="b">
         <v>0</v>
       </c>
       <c r="P198" t="n">
-        <v>4.8</v>
+        <v>298</v>
       </c>
       <c r="Q198" t="b">
         <v>0</v>
       </c>
       <c r="R198" t="inlineStr">
         <is>
-          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
+          <t>SISTEMA MINEIRO DE AVALIAÇÃO E EQUIDADE DA EDUCAÇÃO PÚBLICA - SIMAVE</t>
         </is>
       </c>
       <c r="S198" t="inlineStr">
         <is>
-          <t>Bianual</t>
+          <t>Anual</t>
         </is>
       </c>
       <c r="T198" t="inlineStr">
@@ -18637,7 +18635,7 @@
       </c>
       <c r="U198" t="inlineStr">
         <is>
-          <t>DESEMPENHO NAS AVALIAÇÕES DO SAEB X INDICADOR DE RENDIMENTO</t>
+          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM LÍNGUA PORTUGUESA</t>
         </is>
       </c>
       <c r="V198" t="inlineStr"/>
@@ -18668,7 +18666,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>IDEB ANOS FINAIS DO ENSINO FUNDAMENTAL</t>
+          <t>PROFICIÊNCIA MÉDIA DOS ESTUDANTES DA REDE ESTADUAL NO 5° ANO DO ENSINO FUNDAMENTAL EM MATEMÁTICA (PROEB)</t>
         </is>
       </c>
       <c r="E199" t="b">
@@ -18680,7 +18678,7 @@
         </is>
       </c>
       <c r="G199" t="n">
-        <v>4.6</v>
+        <v>227.2</v>
       </c>
       <c r="H199" t="b">
         <v>0</v>
@@ -18689,37 +18687,37 @@
         <v>45537</v>
       </c>
       <c r="J199" t="n">
-        <v>0</v>
+        <v>242.26</v>
       </c>
       <c r="K199" t="b">
         <v>0</v>
       </c>
       <c r="L199" t="n">
-        <v>6.4</v>
+        <v>250.31</v>
       </c>
       <c r="M199" t="b">
         <v>0</v>
       </c>
       <c r="N199" t="n">
-        <v>0</v>
+        <v>252.7</v>
       </c>
       <c r="O199" t="b">
         <v>0</v>
       </c>
       <c r="P199" t="n">
-        <v>6.6</v>
+        <v>255</v>
       </c>
       <c r="Q199" t="b">
         <v>0</v>
       </c>
       <c r="R199" t="inlineStr">
         <is>
-          <t>INEP - INSTITUTO NACIONAL DE ESTUDOS E PESQUISAS EDUCACIONAIS ANÍSIO TEIXEIRA</t>
+          <t>SISTEMA MINEIRO DE AVALIAÇÃO E EQUIDADE DA EDUCAÇÃO PÚBLICA - SIMAVE</t>
         </is>
       </c>
       <c r="S199" t="inlineStr">
         <is>
-          <t>Bianual</t>
+          <t>Anual</t>
         </is>
       </c>
       <c r="T199" t="inlineStr">
@@ -18729,7 +18727,7 @@
       </c>
       <c r="U199" t="inlineStr">
         <is>
-          <t>DESEMPENHO NAS AVALIAÇÕES DO SAEB X INDICADOR DE RENDIMENTO</t>
+          <t>MÉDIA DA PROFICIÊNCIA DOS ESTUDANTES AVALIADOS EM MATEMÁTICA.</t>
         </is>
       </c>
       <c r="V199" t="inlineStr"/>
@@ -19588,7 +19586,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE ESCOLAS COM MANUTENÇÃO DA CONECTIVIDADE, COM VELOCIDADE MÍNIMA DE CONEXÃO DE ACORDO COM O PADRÃO SEE.</t>
+          <t>PERCENTUAL DE ESCOLAS COM LABORATÓRIO DE INFORMÁTICA EM FUNCIONAMENTO, DE ACORDO COM O PADRÃO SEE/MG</t>
         </is>
       </c>
       <c r="E209" t="b">
@@ -19596,38 +19594,38 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Percentual</t>
+          <t>Porcentagem</t>
         </is>
       </c>
       <c r="G209" t="n">
-        <v>99.90000000000001</v>
+        <v>80</v>
       </c>
       <c r="H209" t="b">
         <v>0</v>
       </c>
       <c r="I209" s="2" t="n">
-        <v>45882</v>
+        <v>44620</v>
       </c>
       <c r="J209" t="n">
-        <v>99.90000000000001</v>
+        <v>90</v>
       </c>
       <c r="K209" t="b">
         <v>0</v>
       </c>
       <c r="L209" t="n">
-        <v>99.90000000000001</v>
+        <v>95</v>
       </c>
       <c r="M209" t="b">
         <v>0</v>
       </c>
       <c r="N209" t="n">
-        <v>99.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O209" t="b">
         <v>0</v>
       </c>
       <c r="P209" t="n">
-        <v>99.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="Q209" t="b">
         <v>0</v>
@@ -19649,7 +19647,7 @@
       </c>
       <c r="U209" t="inlineStr">
         <is>
-          <t>(TOTAL DE ESCOLAS COM O PADRÃO SEE / TOTAL DE ESCOLAS DA REDE) X 100</t>
+          <t>(TOTAL DE ESCOLAS QUE ALCANCEM O NÍVEL DO PADRÃO SEE-MG/TOTAL DE ESCOLAS DA REDE) X 100</t>
         </is>
       </c>
       <c r="V209" t="inlineStr"/>
@@ -19680,7 +19678,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE ESCOLAS COM LABORATÓRIO DE INFORMÁTICA EM FUNCIONAMENTO, DE ACORDO COM O PADRÃO SEE/MG</t>
+          <t>PERCENTUAL DE UNIDADES ESCOLARES COM INFRAESTRUTURA DA SUA REDE FÍSICA AVALIADA COMO BOA OU MUITO BOA</t>
         </is>
       </c>
       <c r="E210" t="b">
@@ -19692,41 +19690,41 @@
         </is>
       </c>
       <c r="G210" t="n">
+        <v>54.15</v>
+      </c>
+      <c r="H210" t="b">
+        <v>0</v>
+      </c>
+      <c r="I210" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="J210" t="n">
+        <v>70</v>
+      </c>
+      <c r="K210" t="b">
+        <v>0</v>
+      </c>
+      <c r="L210" t="n">
+        <v>75</v>
+      </c>
+      <c r="M210" t="b">
+        <v>0</v>
+      </c>
+      <c r="N210" t="n">
         <v>80</v>
       </c>
-      <c r="H210" t="b">
-        <v>0</v>
-      </c>
-      <c r="I210" s="2" t="n">
-        <v>44620</v>
-      </c>
-      <c r="J210" t="n">
-        <v>90</v>
-      </c>
-      <c r="K210" t="b">
-        <v>0</v>
-      </c>
-      <c r="L210" t="n">
-        <v>95</v>
-      </c>
-      <c r="M210" t="b">
-        <v>0</v>
-      </c>
-      <c r="N210" t="n">
-        <v>100</v>
-      </c>
       <c r="O210" t="b">
         <v>0</v>
       </c>
       <c r="P210" t="n">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="Q210" t="b">
         <v>0</v>
       </c>
       <c r="R210" t="inlineStr">
         <is>
-          <t>DIRETORIA DE INFRAESTRUTURA TECNOLÓGICA</t>
+          <t>DIAGNÓSTICO DA INFRAESTRUTURA ESCOLAR</t>
         </is>
       </c>
       <c r="S210" t="inlineStr">
@@ -19741,7 +19739,7 @@
       </c>
       <c r="U210" t="inlineStr">
         <is>
-          <t>(TOTAL DE ESCOLAS QUE ALCANCEM O NÍVEL DO PADRÃO SEE-MG/TOTAL DE ESCOLAS DA REDE) X 100</t>
+          <t>(NÚMERO DE UNIDADES ESCOLARES (ENDEREÇOS) COM INFRAESTRUTURA AVALIADA COMO BOA OU MUITO BOA /NÚMERO TOTAL DE ESCOLAS ESTADUAIS) X 100</t>
         </is>
       </c>
       <c r="V210" t="inlineStr"/>
@@ -19772,7 +19770,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE UNIDADES ESCOLARES COM INFRAESTRUTURA DA SUA REDE FÍSICA AVALIADA COMO BOA OU MUITO BOA</t>
+          <t>PERCENTUAL DE ESCOLAS COM MANUTENÇÃO DA CONECTIVIDADE, COM VELOCIDADE MÍNIMA DE CONEXÃO DE ACORDO COM O PADRÃO SEE.</t>
         </is>
       </c>
       <c r="E211" t="b">
@@ -19780,45 +19778,45 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>Porcentagem</t>
+          <t>Percentual</t>
         </is>
       </c>
       <c r="G211" t="n">
-        <v>54.15</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="H211" t="b">
         <v>0</v>
       </c>
       <c r="I211" s="2" t="n">
-        <v>45688</v>
+        <v>45882</v>
       </c>
       <c r="J211" t="n">
-        <v>70</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="K211" t="b">
         <v>0</v>
       </c>
       <c r="L211" t="n">
-        <v>75</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="M211" t="b">
         <v>0</v>
       </c>
       <c r="N211" t="n">
-        <v>80</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="O211" t="b">
         <v>0</v>
       </c>
       <c r="P211" t="n">
-        <v>81</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="Q211" t="b">
         <v>0</v>
       </c>
       <c r="R211" t="inlineStr">
         <is>
-          <t>DIAGNÓSTICO DA INFRAESTRUTURA ESCOLAR</t>
+          <t>DIRETORIA DE INFRAESTRUTURA TECNOLÓGICA</t>
         </is>
       </c>
       <c r="S211" t="inlineStr">
@@ -19833,7 +19831,7 @@
       </c>
       <c r="U211" t="inlineStr">
         <is>
-          <t>(NÚMERO DE UNIDADES ESCOLARES (ENDEREÇOS) COM INFRAESTRUTURA AVALIADA COMO BOA OU MUITO BOA /NÚMERO TOTAL DE ESCOLAS ESTADUAIS) X 100</t>
+          <t>(TOTAL DE ESCOLAS COM O PADRÃO SEE / TOTAL DE ESCOLAS DA REDE) X 100</t>
         </is>
       </c>
       <c r="V211" t="inlineStr"/>
@@ -19956,7 +19954,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE EXECUÇÃO DE CONVÊNIOS FIRMADOS COM OS MUNICÍPIO CUJO OJBETO SEJA AQUISIÇÃO DE BENS PERMANENTES</t>
+          <t>PERCENTUAL DE ESTUDANTES RESIDENTES EM ÁREAS RURAIS DA EDUCAÇÃO BÁSICA DA REDE ESTADUAL DE ENSINO ATENDIDOS NO PROGRAMA DE TRANSPORTE DO ESCOLAR (PTE)</t>
         </is>
       </c>
       <c r="E213" t="b">
@@ -19967,19 +19965,23 @@
           <t>%</t>
         </is>
       </c>
-      <c r="G213" t="inlineStr"/>
+      <c r="G213" t="n">
+        <v>100</v>
+      </c>
       <c r="H213" t="b">
-        <v>1</v>
-      </c>
-      <c r="I213" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I213" s="2" t="n">
+        <v>45291</v>
+      </c>
       <c r="J213" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="K213" t="b">
         <v>0</v>
       </c>
       <c r="L213" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M213" t="b">
         <v>0</v>
@@ -19998,7 +20000,7 @@
       </c>
       <c r="R213" t="inlineStr">
         <is>
-          <t>SIGCON</t>
+          <t>SEE</t>
         </is>
       </c>
       <c r="S213" t="inlineStr">
@@ -20013,24 +20015,16 @@
       </c>
       <c r="U213" t="inlineStr">
         <is>
-          <t>NÚMERO DE CONVÊNIOS ENCERRADOS COM OBJETO CONCLUÍDO DIVIDO PELO NÚMERO TOTAL DE CONVÊNIOS FIRMADOS.</t>
-        </is>
-      </c>
-      <c r="V213" t="inlineStr">
-        <is>
-          <t>ORGANIZAÇÃO, ESTRUTURA E DEFINIÇÃO DO FLUXO DO PROGRAMA FOI ESTABELECIDO EM JUNHO/2025. CRIAÇÃO DO PAINEL COM A CONSOLIDAÇÃO DOS DADOS PARA DAR MAIS TRANSPARÊNCIA E DIVULGAÇÃO DOS DADOS.</t>
-        </is>
-      </c>
-      <c r="W213" t="inlineStr">
-        <is>
-          <t>ORGANIZAÇÃO, ESTRUTURA E DEFINIÇÃO DO FLUXO DO PROGRAMA FOI ESTABELECIDO EM JUNHO/2025. CRIAÇÃO DO PAINEL COM A CONSOLIDAÇÃO DOS DADOS PARA DAR MAIS TRANSPARÊNCIA E DIVULGAÇÃO DOS DADOS.</t>
-        </is>
-      </c>
+          <t>(NÚMERO DE ESTUDANTES RESIDENTES EM ÁREAS RURAIS DA EDUCAÇÃO BÁSICA DA REDE ESTADUAL DE ENSINO ATENDIDOS / NÚMERO DE ESTUDANTES RESIDENTES EM ÁREAS RURAIS DA EDUCAÇÃO BÁSICA DA REDE ESTADUAL DE ENSINO) * 100</t>
+        </is>
+      </c>
+      <c r="V213" t="inlineStr"/>
+      <c r="W213" t="inlineStr"/>
       <c r="X213" s="2" t="n">
         <v>45917.58680555555</v>
       </c>
       <c r="Y213" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z213" t="inlineStr">
         <is>
@@ -20052,7 +20046,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE OBRAS CONCLUÍDAS COM RECURSOS DO PROGRAMA</t>
+          <t>PERCENTUAL DE EXECUÇÃO DE CONVÊNIOS FIRMADOS COM OS MUNICÍPIO CUJO OJBETO SEJA AQUISIÇÃO DE BENS PERMANENTES</t>
         </is>
       </c>
       <c r="E214" t="b">
@@ -20094,7 +20088,7 @@
       </c>
       <c r="R214" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE PAGAMENTOS REALIZADOS - CONTROLE PRÓPRIO</t>
+          <t>SIGCON</t>
         </is>
       </c>
       <c r="S214" t="inlineStr">
@@ -20109,7 +20103,7 @@
       </c>
       <c r="U214" t="inlineStr">
         <is>
-          <t>VALOR TOTAL DO RECURSO EXECUTADO DIVIDIDO PELO VALOR TOTAL DO RECURSO DISPONIBILIZADO NO ANO</t>
+          <t>NÚMERO DE CONVÊNIOS ENCERRADOS COM OBJETO CONCLUÍDO DIVIDO PELO NÚMERO TOTAL DE CONVÊNIOS FIRMADOS.</t>
         </is>
       </c>
       <c r="V214" t="inlineStr">
@@ -20148,7 +20142,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE ESTUDANTES RESIDENTES EM ÁREAS RURAIS DA EDUCAÇÃO BÁSICA DA REDE ESTADUAL DE ENSINO ATENDIDOS NO PROGRAMA DE TRANSPORTE DO ESCOLAR (PTE)</t>
+          <t>PERCENTUAL DE OBRAS CONCLUÍDAS COM RECURSOS DO PROGRAMA</t>
         </is>
       </c>
       <c r="E215" t="b">
@@ -20159,23 +20153,19 @@
           <t>%</t>
         </is>
       </c>
-      <c r="G215" t="n">
-        <v>100</v>
-      </c>
+      <c r="G215" t="inlineStr"/>
       <c r="H215" t="b">
-        <v>0</v>
-      </c>
-      <c r="I215" s="2" t="n">
-        <v>45291</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I215" t="inlineStr"/>
       <c r="J215" t="n">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K215" t="b">
         <v>0</v>
       </c>
       <c r="L215" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="M215" t="b">
         <v>0</v>
@@ -20194,7 +20184,7 @@
       </c>
       <c r="R215" t="inlineStr">
         <is>
-          <t>SEE</t>
+          <t>PERCENTUAL DE PAGAMENTOS REALIZADOS - CONTROLE PRÓPRIO</t>
         </is>
       </c>
       <c r="S215" t="inlineStr">
@@ -20209,16 +20199,24 @@
       </c>
       <c r="U215" t="inlineStr">
         <is>
-          <t>(NÚMERO DE ESTUDANTES RESIDENTES EM ÁREAS RURAIS DA EDUCAÇÃO BÁSICA DA REDE ESTADUAL DE ENSINO ATENDIDOS / NÚMERO DE ESTUDANTES RESIDENTES EM ÁREAS RURAIS DA EDUCAÇÃO BÁSICA DA REDE ESTADUAL DE ENSINO) * 100</t>
-        </is>
-      </c>
-      <c r="V215" t="inlineStr"/>
-      <c r="W215" t="inlineStr"/>
+          <t>VALOR TOTAL DO RECURSO EXECUTADO DIVIDIDO PELO VALOR TOTAL DO RECURSO DISPONIBILIZADO NO ANO</t>
+        </is>
+      </c>
+      <c r="V215" t="inlineStr">
+        <is>
+          <t>ORGANIZAÇÃO, ESTRUTURA E DEFINIÇÃO DO FLUXO DO PROGRAMA FOI ESTABELECIDO EM JUNHO/2025. CRIAÇÃO DO PAINEL COM A CONSOLIDAÇÃO DOS DADOS PARA DAR MAIS TRANSPARÊNCIA E DIVULGAÇÃO DOS DADOS.</t>
+        </is>
+      </c>
+      <c r="W215" t="inlineStr">
+        <is>
+          <t>ORGANIZAÇÃO, ESTRUTURA E DEFINIÇÃO DO FLUXO DO PROGRAMA FOI ESTABELECIDO EM JUNHO/2025. CRIAÇÃO DO PAINEL COM A CONSOLIDAÇÃO DOS DADOS PARA DAR MAIS TRANSPARÊNCIA E DIVULGAÇÃO DOS DADOS.</t>
+        </is>
+      </c>
       <c r="X215" s="2" t="n">
         <v>45917.58680555555</v>
       </c>
       <c r="Y215" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z215" t="inlineStr">
         <is>
@@ -20332,7 +20330,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE COMARCAS QUE CONTAM COM A PRESENÇA DA DEFENSORIA PÚBLICA</t>
+          <t>NÚMERO DE DEFENSORES PÚBLICOS POR 100.000 HABITANTES</t>
         </is>
       </c>
       <c r="E217" t="b">
@@ -20340,11 +20338,11 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>%</t>
+          <t>Defensores por 100 mil habitantes</t>
         </is>
       </c>
       <c r="G217" t="n">
-        <v>38.59</v>
+        <v>3.4</v>
       </c>
       <c r="H217" t="b">
         <v>0</v>
@@ -20353,25 +20351,25 @@
         <v>45869</v>
       </c>
       <c r="J217" t="n">
-        <v>38.59</v>
+        <v>3.39</v>
       </c>
       <c r="K217" t="b">
         <v>0</v>
       </c>
       <c r="L217" t="n">
-        <v>38.59</v>
+        <v>3.38</v>
       </c>
       <c r="M217" t="b">
         <v>0</v>
       </c>
       <c r="N217" t="n">
-        <v>38.59</v>
+        <v>3.37</v>
       </c>
       <c r="O217" t="b">
         <v>0</v>
       </c>
       <c r="P217" t="n">
-        <v>38.59</v>
+        <v>3.36</v>
       </c>
       <c r="Q217" t="b">
         <v>0</v>
@@ -20393,7 +20391,7 @@
       </c>
       <c r="U217" t="inlineStr">
         <is>
-          <t>(NÚMERO DE COMARCAS QUE CONTAM COM A PRESENÇA DA DEFENSORIA PÚBLICA/NÚMERO DE COMARCAS EXISTENTES NO ESTADO DE MINAS GERAIS)*100</t>
+          <t>(NÚMERO DE DEFENSORES PÚBLICOS/POPULAÇÃO DO ESTADO DE MINAS GERAIS)*100.000</t>
         </is>
       </c>
       <c r="V217" t="inlineStr"/>
@@ -20424,7 +20422,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE COMARCAS QUE SE ENCONTRAM TOTALMENTE PROVIDAS DE DEFENSORES PÚBLICOS</t>
+          <t>NÚMERO DE PRESTAÇÕES JURÍDICAS POR 100.000 HABITANTES</t>
         </is>
       </c>
       <c r="E218" t="b">
@@ -20432,11 +20430,11 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>%</t>
+          <t>prestação jurídica por 100 mil habitantes</t>
         </is>
       </c>
       <c r="G218" t="n">
-        <v>11.07</v>
+        <v>20387.33</v>
       </c>
       <c r="H218" t="b">
         <v>0</v>
@@ -20445,32 +20443,32 @@
         <v>45869</v>
       </c>
       <c r="J218" t="n">
-        <v>11.07</v>
+        <v>34838.58</v>
       </c>
       <c r="K218" t="b">
         <v>0</v>
       </c>
       <c r="L218" t="n">
-        <v>11.07</v>
+        <v>34736.42</v>
       </c>
       <c r="M218" t="b">
         <v>0</v>
       </c>
       <c r="N218" t="n">
-        <v>11.07</v>
+        <v>34640.66</v>
       </c>
       <c r="O218" t="b">
         <v>0</v>
       </c>
       <c r="P218" t="n">
-        <v>11.07</v>
+        <v>34550.91</v>
       </c>
       <c r="Q218" t="b">
         <v>0</v>
       </c>
       <c r="R218" t="inlineStr">
         <is>
-          <t>DEFENSORIA PÚBICA DO ESTADO DE MINAS GERAIS</t>
+          <t>DEFENSORIA PÚBLICA DO ESTADO DE  MINAS GERAIS</t>
         </is>
       </c>
       <c r="S218" t="inlineStr">
@@ -20485,7 +20483,7 @@
       </c>
       <c r="U218" t="inlineStr">
         <is>
-          <t>(SOMATÓRIO DE COMARCAS TOTALMENTE PROVIDAS DE DEFENSORES PÚBLICOS/TOTAL DE COMARCAS DO ESTADO DE MINAS GERAIS)*100</t>
+          <t>(NÚMERO DE PRESTAÇÕES JURÍDICAS/POPULAÇÃO DO ESTADO DE MINAS GERAIS)*100.000.</t>
         </is>
       </c>
       <c r="V218" t="inlineStr"/>
@@ -20516,7 +20514,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>NÚMERO DE DEFENSORES PÚBLICOS POR 100.000 HABITANTES</t>
+          <t>PERCENTUAL DE COMARCAS QUE CONTAM COM A PRESENÇA DA DEFENSORIA PÚBLICA</t>
         </is>
       </c>
       <c r="E219" t="b">
@@ -20524,11 +20522,11 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>Defensores por 100 mil habitantes</t>
+          <t>%</t>
         </is>
       </c>
       <c r="G219" t="n">
-        <v>3.4</v>
+        <v>38.59</v>
       </c>
       <c r="H219" t="b">
         <v>0</v>
@@ -20537,25 +20535,25 @@
         <v>45869</v>
       </c>
       <c r="J219" t="n">
-        <v>3.39</v>
+        <v>38.59</v>
       </c>
       <c r="K219" t="b">
         <v>0</v>
       </c>
       <c r="L219" t="n">
-        <v>3.38</v>
+        <v>38.59</v>
       </c>
       <c r="M219" t="b">
         <v>0</v>
       </c>
       <c r="N219" t="n">
-        <v>3.37</v>
+        <v>38.59</v>
       </c>
       <c r="O219" t="b">
         <v>0</v>
       </c>
       <c r="P219" t="n">
-        <v>3.36</v>
+        <v>38.59</v>
       </c>
       <c r="Q219" t="b">
         <v>0</v>
@@ -20577,7 +20575,7 @@
       </c>
       <c r="U219" t="inlineStr">
         <is>
-          <t>(NÚMERO DE DEFENSORES PÚBLICOS/POPULAÇÃO DO ESTADO DE MINAS GERAIS)*100.000</t>
+          <t>(NÚMERO DE COMARCAS QUE CONTAM COM A PRESENÇA DA DEFENSORIA PÚBLICA/NÚMERO DE COMARCAS EXISTENTES NO ESTADO DE MINAS GERAIS)*100</t>
         </is>
       </c>
       <c r="V219" t="inlineStr"/>
@@ -20608,7 +20606,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>NÚMERO DE PRESTAÇÕES JURÍDICAS POR 100.000 HABITANTES</t>
+          <t>PERCENTUAL DE COMARCAS QUE SE ENCONTRAM TOTALMENTE PROVIDAS DE DEFENSORES PÚBLICOS</t>
         </is>
       </c>
       <c r="E220" t="b">
@@ -20616,11 +20614,11 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>prestação jurídica por 100 mil habitantes</t>
+          <t>%</t>
         </is>
       </c>
       <c r="G220" t="n">
-        <v>20387.33</v>
+        <v>11.07</v>
       </c>
       <c r="H220" t="b">
         <v>0</v>
@@ -20629,32 +20627,32 @@
         <v>45869</v>
       </c>
       <c r="J220" t="n">
-        <v>34838.58</v>
+        <v>11.07</v>
       </c>
       <c r="K220" t="b">
         <v>0</v>
       </c>
       <c r="L220" t="n">
-        <v>34736.42</v>
+        <v>11.07</v>
       </c>
       <c r="M220" t="b">
         <v>0</v>
       </c>
       <c r="N220" t="n">
-        <v>34640.66</v>
+        <v>11.07</v>
       </c>
       <c r="O220" t="b">
         <v>0</v>
       </c>
       <c r="P220" t="n">
-        <v>34550.91</v>
+        <v>11.07</v>
       </c>
       <c r="Q220" t="b">
         <v>0</v>
       </c>
       <c r="R220" t="inlineStr">
         <is>
-          <t>DEFENSORIA PÚBLICA DO ESTADO DE  MINAS GERAIS</t>
+          <t>DEFENSORIA PÚBICA DO ESTADO DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="S220" t="inlineStr">
@@ -20669,7 +20667,7 @@
       </c>
       <c r="U220" t="inlineStr">
         <is>
-          <t>(NÚMERO DE PRESTAÇÕES JURÍDICAS/POPULAÇÃO DO ESTADO DE MINAS GERAIS)*100.000.</t>
+          <t>(SOMATÓRIO DE COMARCAS TOTALMENTE PROVIDAS DE DEFENSORES PÚBLICOS/TOTAL DE COMARCAS DO ESTADO DE MINAS GERAIS)*100</t>
         </is>
       </c>
       <c r="V220" t="inlineStr"/>
@@ -20700,7 +20698,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>VOLUME DE RECURSOS PÚBLICOS AFETOS A PROCESSOS LICITATÓRIOS SUBMETIDOS À FISCALIZAÇÃO POR MEIO DE TRILHAS ELETRÔNICAS</t>
+          <t>ÍNDICE DE DELIBERAÇÃO DE PROCESSOS DE ATOS DE PESSOAL COM ANO REFERÊNCIA A PARTIR DE 2021</t>
         </is>
       </c>
       <c r="E221" t="b">
@@ -20708,11 +20706,11 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>bilhões de Reais (R$)</t>
+          <t>%</t>
         </is>
       </c>
       <c r="G221" t="n">
-        <v>14.4</v>
+        <v>96.59</v>
       </c>
       <c r="H221" t="b">
         <v>0</v>
@@ -20721,25 +20719,25 @@
         <v>45657</v>
       </c>
       <c r="J221" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
       </c>
       <c r="L221" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="M221" t="b">
         <v>0</v>
       </c>
       <c r="N221" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="O221" t="b">
         <v>0</v>
       </c>
       <c r="P221" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="Q221" t="b">
         <v>0</v>
@@ -20761,7 +20759,7 @@
       </c>
       <c r="U221" t="inlineStr">
         <is>
-          <t>VALOR, EM BILHÕES DE REAIS, DA SOMA DOS RECURSOS ENVOLVIDOS NOS PROCESSOS LICITATÓRIOS ANALISADOS NAS TRILHAS ELETRÔNICAS DE FISCALIZAÇÃO</t>
+          <t>(NÚMERO DE PROCESSOS DE ATOS DE PESSOAL CONCESSÓRIOS DELIBERADOS, COM ANO DE REFERÊNCIA DOS ÚLTIMOS 6 EXERCÍCIOS (2021 A 2026) / NÚMERO DE PROCESSOS DE ATOS DE PESSOAL CONCESSORIOS AUTUADOS NO EXERCÍCIO ANTERIOR 2025) * 100</t>
         </is>
       </c>
       <c r="V221" t="inlineStr"/>
@@ -20792,7 +20790,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>ÍNDICE DE DELIBERAÇÃO DE PROCESSOS DE ATOS DE PESSOAL COM ANO REFERÊNCIA A PARTIR DE 2021</t>
+          <t>ÍNDICE DE DELIBERAÇÃO DE PROCESSOS  DE PCA E PEDIDO DE REEXAME, PARA TODOS OS ANOS REFERÊNCIA, E DE DEMAIS NATUREZAS, COM ANO REFERÊNCIA A PARTIR DE 2021.</t>
         </is>
       </c>
       <c r="E222" t="b">
@@ -20804,7 +20802,7 @@
         </is>
       </c>
       <c r="G222" t="n">
-        <v>96.59</v>
+        <v>80.42</v>
       </c>
       <c r="H222" t="b">
         <v>0</v>
@@ -20813,25 +20811,25 @@
         <v>45657</v>
       </c>
       <c r="J222" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="K222" t="b">
         <v>0</v>
       </c>
       <c r="L222" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="M222" t="b">
         <v>0</v>
       </c>
       <c r="N222" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="O222" t="b">
         <v>0</v>
       </c>
       <c r="P222" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="Q222" t="b">
         <v>0</v>
@@ -20853,7 +20851,7 @@
       </c>
       <c r="U222" t="inlineStr">
         <is>
-          <t>(NÚMERO DE PROCESSOS DE ATOS DE PESSOAL CONCESSÓRIOS DELIBERADOS, COM ANO DE REFERÊNCIA DOS ÚLTIMOS 6 EXERCÍCIOS (2021 A 2026) / NÚMERO DE PROCESSOS DE ATOS DE PESSOAL CONCESSORIOS AUTUADOS NO EXERCÍCIO ANTERIOR 2025) * 100</t>
+          <t>[(NÚMERO DE PROCESSOS DELIBERADOS DE PCA E PEDIDO DE REEXAME TODOS OS ANOS  REFERÊNCIA) + (NÚMERO DE PROCESSOS DELIBERADOS DE DEMAIS NATUREZAS COM ANO DE REFERÊNCIA DOS ÚLTIMOS 6 EXERCÍCIOS (2021 A 2026) / NÚMERO DE PROCESSOS DE PCA, PEDIDO DE REEXAME E DEMAIS NATUREZAS AUTUADOS NO EXERCÍCIO DE 2025] *100</t>
         </is>
       </c>
       <c r="V222" t="inlineStr"/>
@@ -20884,7 +20882,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>ÍNDICE DE DELIBERAÇÃO DE PROCESSOS  DE PCA E PEDIDO DE REEXAME, PARA TODOS OS ANOS REFERÊNCIA, E DE DEMAIS NATUREZAS, COM ANO REFERÊNCIA A PARTIR DE 2021.</t>
+          <t>ÍNDICE DE CUMPRIMENTO DO PLANO ANUAL DE FISCALIZAÇÃO.</t>
         </is>
       </c>
       <c r="E223" t="b">
@@ -20896,7 +20894,7 @@
         </is>
       </c>
       <c r="G223" t="n">
-        <v>80.42</v>
+        <v>93.70999999999999</v>
       </c>
       <c r="H223" t="b">
         <v>0</v>
@@ -20905,32 +20903,32 @@
         <v>45657</v>
       </c>
       <c r="J223" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K223" t="b">
         <v>0</v>
       </c>
       <c r="L223" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M223" t="b">
         <v>0</v>
       </c>
       <c r="N223" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="O223" t="b">
         <v>0</v>
       </c>
       <c r="P223" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="Q223" t="b">
         <v>0</v>
       </c>
       <c r="R223" t="inlineStr">
         <is>
-          <t>TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS</t>
+          <t>SUPERINTENDÊNCIA DE CONTROLE EXTERNO</t>
         </is>
       </c>
       <c r="S223" t="inlineStr">
@@ -20945,7 +20943,7 @@
       </c>
       <c r="U223" t="inlineStr">
         <is>
-          <t>[(NÚMERO DE PROCESSOS DELIBERADOS DE PCA E PEDIDO DE REEXAME TODOS OS ANOS  REFERÊNCIA) + (NÚMERO DE PROCESSOS DELIBERADOS DE DEMAIS NATUREZAS COM ANO DE REFERÊNCIA DOS ÚLTIMOS 6 EXERCÍCIOS (2021 A 2026) / NÚMERO DE PROCESSOS DE PCA, PEDIDO DE REEXAME E DEMAIS NATUREZAS AUTUADOS NO EXERCÍCIO DE 2025] *100</t>
+          <t>(PONTOS TOTAIS OBTIDOS / PONTOS TOTAIS POSSÍVEIS DE OBTER) X 100.</t>
         </is>
       </c>
       <c r="V223" t="inlineStr"/>
@@ -20976,7 +20974,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>ÍNDICE DE CUMPRIMENTO DO PLANO ANUAL DE FISCALIZAÇÃO.</t>
+          <t>ÍNDICE DE PROCESSOS DE AUDITORIAS DELIBERADOS NO PRAZO DE 360 DIAS DA AUTUAÇÃO, EM RELAÇÃO AO TOTAL DE AUDITORIAS AUTUADAS NO ANO ANTERIOR</t>
         </is>
       </c>
       <c r="E224" t="b">
@@ -20988,7 +20986,7 @@
         </is>
       </c>
       <c r="G224" t="n">
-        <v>93.70999999999999</v>
+        <v>42.31</v>
       </c>
       <c r="H224" t="b">
         <v>0</v>
@@ -20997,32 +20995,32 @@
         <v>45657</v>
       </c>
       <c r="J224" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="K224" t="b">
         <v>0</v>
       </c>
       <c r="L224" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="M224" t="b">
         <v>0</v>
       </c>
       <c r="N224" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="O224" t="b">
         <v>0</v>
       </c>
       <c r="P224" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="Q224" t="b">
         <v>0</v>
       </c>
       <c r="R224" t="inlineStr">
         <is>
-          <t>SUPERINTENDÊNCIA DE CONTROLE EXTERNO</t>
+          <t>TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="S224" t="inlineStr">
@@ -21037,7 +21035,7 @@
       </c>
       <c r="U224" t="inlineStr">
         <is>
-          <t>(PONTOS TOTAIS OBTIDOS / PONTOS TOTAIS POSSÍVEIS DE OBTER) X 100.</t>
+          <t>(NÚMERO DE PROCESSOS DE AUDITORIAS DELIBERADOS NO PRAZO DE 360 DIAS DA AUTUAÇÃO / TOTAL DE PROCESSOS DE AUDITORIAS AUTUADOS EM 2025) *100</t>
         </is>
       </c>
       <c r="V224" t="inlineStr"/>
@@ -21068,7 +21066,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>ÍNDICE DE PROCESSOS DE AUDITORIAS DELIBERADOS NO PRAZO DE 360 DIAS DA AUTUAÇÃO, EM RELAÇÃO AO TOTAL DE AUDITORIAS AUTUADAS NO ANO ANTERIOR</t>
+          <t>PERCENTUAL DE MUNICÍPIOS ABRANGIDOS PELAS AÇÕES DE FISCALIZAÇÃO PRESENCIAIS OU MEDIANTE TRILHAS ELETRÔNICAS</t>
         </is>
       </c>
       <c r="E225" t="b">
@@ -21080,7 +21078,7 @@
         </is>
       </c>
       <c r="G225" t="n">
-        <v>42.31</v>
+        <v>100</v>
       </c>
       <c r="H225" t="b">
         <v>0</v>
@@ -21089,25 +21087,25 @@
         <v>45657</v>
       </c>
       <c r="J225" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="K225" t="b">
         <v>0</v>
       </c>
       <c r="L225" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="M225" t="b">
         <v>0</v>
       </c>
       <c r="N225" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O225" t="b">
         <v>0</v>
       </c>
       <c r="P225" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="Q225" t="b">
         <v>0</v>
@@ -21129,7 +21127,7 @@
       </c>
       <c r="U225" t="inlineStr">
         <is>
-          <t>(NÚMERO DE PROCESSOS DE AUDITORIAS DELIBERADOS NO PRAZO DE 360 DIAS DA AUTUAÇÃO / TOTAL DE PROCESSOS DE AUDITORIAS AUTUADOS EM 2025) *100</t>
+          <t>(NÚMERO DE MUNICÍPIOS ABRANGIDOS PELAS AÇÕES DE FISCALIZAÇÃO PRESENCAIS OU MEDIANTE TRILHAS ELETRÔNICAS / NÚMERO DE MUNICÍPIOS DO ESTADO) *100</t>
         </is>
       </c>
       <c r="V225" t="inlineStr"/>
@@ -21160,7 +21158,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE MUNICÍPIOS ABRANGIDOS PELAS AÇÕES DE FISCALIZAÇÃO PRESENCIAIS OU MEDIANTE TRILHAS ELETRÔNICAS</t>
+          <t>PERCENTUAL DE AÇÕES DE FISCALIZAÇÃO PREVISTAS NO PLANO ANUAL DE FISCALIZAÇÃO - PAF ALINHADAS AOS OBJETIVOS DE DESENVOLVIMENTO SUSTENTÁVEL - ODS</t>
         </is>
       </c>
       <c r="E226" t="b">
@@ -21221,7 +21219,7 @@
       </c>
       <c r="U226" t="inlineStr">
         <is>
-          <t>(NÚMERO DE MUNICÍPIOS ABRANGIDOS PELAS AÇÕES DE FISCALIZAÇÃO PRESENCAIS OU MEDIANTE TRILHAS ELETRÔNICAS / NÚMERO DE MUNICÍPIOS DO ESTADO) *100</t>
+          <t>(NÚMERO DE AÇÕES DE FISCALIZAÇÃO PREVISTAS NO PAF ALINHADAS AOS OBJETIVOS DE DESENVOLVIMENTO SUSTENTÁVEL-ODS / NÚMERO TOTAL DE AÇÕES DE FISCALIZAÇÃO PREVISTAS PAF) *100</t>
         </is>
       </c>
       <c r="V226" t="inlineStr"/>
@@ -21252,7 +21250,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE AÇÕES DE FISCALIZAÇÃO PREVISTAS NO PLANO ANUAL DE FISCALIZAÇÃO - PAF ALINHADAS AOS OBJETIVOS DE DESENVOLVIMENTO SUSTENTÁVEL - ODS</t>
+          <t>ÍNDICE DE IRREGULARIDADES SANADAS OU EVITADAS EM PROCESSOS LICITATÓRIOS DISPENSANDO A FORMALIZAÇÃO DE PROCESSO</t>
         </is>
       </c>
       <c r="E227" t="b">
@@ -21263,35 +21261,31 @@
           <t>%</t>
         </is>
       </c>
-      <c r="G227" t="n">
-        <v>100</v>
-      </c>
+      <c r="G227" t="inlineStr"/>
       <c r="H227" t="b">
-        <v>0</v>
-      </c>
-      <c r="I227" s="2" t="n">
-        <v>45657</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I227" t="inlineStr"/>
       <c r="J227" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K227" t="b">
         <v>0</v>
       </c>
       <c r="L227" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="M227" t="b">
         <v>0</v>
       </c>
       <c r="N227" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="O227" t="b">
         <v>0</v>
       </c>
       <c r="P227" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="Q227" t="b">
         <v>0</v>
@@ -21313,11 +21307,15 @@
       </c>
       <c r="U227" t="inlineStr">
         <is>
-          <t>(NÚMERO DE AÇÕES DE FISCALIZAÇÃO PREVISTAS NO PAF ALINHADAS AOS OBJETIVOS DE DESENVOLVIMENTO SUSTENTÁVEL-ODS / NÚMERO TOTAL DE AÇÕES DE FISCALIZAÇÃO PREVISTAS PAF) *100</t>
+          <t>PERCENTUAL DE IRREGULARIDADES EM PROCESSOS LICITATÓRIOS SANADAS OU EVITADAS DISPENSANDO A FORMALIZAÇÃO DE PROCESSO, POR MEIO DE AÇÕES DE INTELIGÊNCIA OU DE ANÁLISE DE DADOS</t>
         </is>
       </c>
       <c r="V227" t="inlineStr"/>
-      <c r="W227" t="inlineStr"/>
+      <c r="W227" t="inlineStr">
+        <is>
+          <t>O PRIMEIRO EXERCÍCIO DO INDICADOR SERÁ 2026.</t>
+        </is>
+      </c>
       <c r="X227" s="2" t="n">
         <v>45922.63333333333</v>
       </c>
@@ -21344,7 +21342,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>ÍNDICE DE IRREGULARIDADES SANADAS OU EVITADAS EM PROCESSOS LICITATÓRIOS DISPENSANDO A FORMALIZAÇÃO DE PROCESSO</t>
+          <t>QUANTIDADE DE INDÍCIOS DE IRREGULARIDADE EM TRILHAS DE ATOS DE PESSOAL DECORRENTES DE CRUZAMENTO DE DADOS E LEVADAS AO CONHECIMENTO DOS JURISDICIONADOS</t>
         </is>
       </c>
       <c r="E228" t="b">
@@ -21352,7 +21350,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>%</t>
+          <t>UNIDADE</t>
         </is>
       </c>
       <c r="G228" t="inlineStr"/>
@@ -21361,32 +21359,32 @@
       </c>
       <c r="I228" t="inlineStr"/>
       <c r="J228" t="n">
-        <v>75</v>
+        <v>7000</v>
       </c>
       <c r="K228" t="b">
         <v>0</v>
       </c>
       <c r="L228" t="n">
-        <v>75</v>
+        <v>7000</v>
       </c>
       <c r="M228" t="b">
         <v>0</v>
       </c>
       <c r="N228" t="n">
-        <v>75</v>
+        <v>7000</v>
       </c>
       <c r="O228" t="b">
         <v>0</v>
       </c>
       <c r="P228" t="n">
-        <v>75</v>
+        <v>7000</v>
       </c>
       <c r="Q228" t="b">
         <v>0</v>
       </c>
       <c r="R228" t="inlineStr">
         <is>
-          <t>TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS</t>
+          <t>TRIBUNAL DE CONTAS DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="S228" t="inlineStr">
@@ -21401,13 +21399,13 @@
       </c>
       <c r="U228" t="inlineStr">
         <is>
-          <t>PERCENTUAL DE IRREGULARIDADES EM PROCESSOS LICITATÓRIOS SANADAS OU EVITADAS DISPENSANDO A FORMALIZAÇÃO DE PROCESSO, POR MEIO DE AÇÕES DE INTELIGÊNCIA OU DE ANÁLISE DE DADOS</t>
+          <t>NÚMERO ABSOLUTO DE INDÍCIOS DE IRREGULARIDADE EM TRILHAS DE ATOS DE PESSOAL DECORRENTES DO CRUZAMENTO DE DADOS QUE FORAM LEVADOS AO CONHECIMENTO DOS JURISDICIONADOS</t>
         </is>
       </c>
       <c r="V228" t="inlineStr"/>
       <c r="W228" t="inlineStr">
         <is>
-          <t>O PRIMEIRO EXERCÍCIO DO INDICADOR SERÁ 2026.</t>
+          <t>O INDICADOR FOI ALTERADO EM SUA REDAÇÃO PARA MAIOR QUALIFICAÇÃO DAS AÇÕES DE CONTROLE, PORTANTOO PRIMEIRO EXERCÍCIO DE REFERÊNCIA SERÁ 2026.</t>
         </is>
       </c>
       <c r="X228" s="2" t="n">
@@ -21802,7 +21800,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>QUANTIDADE DE INDÍCIOS DE IRREGULARIDADE EM TRILHAS DE ATOS DE PESSOAL DECORRENTES DE CRUZAMENTO DE DADOS E LEVADAS AO CONHECIMENTO DOS JURISDICIONADOS</t>
+          <t>VOLUME DE RECURSOS PÚBLICOS AFETOS A PROCESSOS LICITATÓRIOS SUBMETIDOS À FISCALIZAÇÃO POR MEIO DE TRILHAS ELETRÔNICAS</t>
         </is>
       </c>
       <c r="E233" t="b">
@@ -21810,41 +21808,45 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>UNIDADE</t>
-        </is>
-      </c>
-      <c r="G233" t="inlineStr"/>
+          <t>bilhões de Reais (R$)</t>
+        </is>
+      </c>
+      <c r="G233" t="n">
+        <v>14.4</v>
+      </c>
       <c r="H233" t="b">
-        <v>1</v>
-      </c>
-      <c r="I233" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I233" s="2" t="n">
+        <v>45657</v>
+      </c>
       <c r="J233" t="n">
-        <v>7000</v>
+        <v>15</v>
       </c>
       <c r="K233" t="b">
         <v>0</v>
       </c>
       <c r="L233" t="n">
-        <v>7000</v>
+        <v>15</v>
       </c>
       <c r="M233" t="b">
         <v>0</v>
       </c>
       <c r="N233" t="n">
-        <v>7000</v>
+        <v>15</v>
       </c>
       <c r="O233" t="b">
         <v>0</v>
       </c>
       <c r="P233" t="n">
-        <v>7000</v>
+        <v>15</v>
       </c>
       <c r="Q233" t="b">
         <v>0</v>
       </c>
       <c r="R233" t="inlineStr">
         <is>
-          <t>TRIBUNAL DE CONTAS DE MINAS GERAIS</t>
+          <t>TRIBUNAL DE CONTAS DO ESTADO DE MINAS GERAIS</t>
         </is>
       </c>
       <c r="S233" t="inlineStr">
@@ -21859,15 +21861,11 @@
       </c>
       <c r="U233" t="inlineStr">
         <is>
-          <t>NÚMERO ABSOLUTO DE INDÍCIOS DE IRREGULARIDADE EM TRILHAS DE ATOS DE PESSOAL DECORRENTES DO CRUZAMENTO DE DADOS QUE FORAM LEVADOS AO CONHECIMENTO DOS JURISDICIONADOS</t>
+          <t>VALOR, EM BILHÕES DE REAIS, DA SOMA DOS RECURSOS ENVOLVIDOS NOS PROCESSOS LICITATÓRIOS ANALISADOS NAS TRILHAS ELETRÔNICAS DE FISCALIZAÇÃO</t>
         </is>
       </c>
       <c r="V233" t="inlineStr"/>
-      <c r="W233" t="inlineStr">
-        <is>
-          <t>O INDICADOR FOI ALTERADO EM SUA REDAÇÃO PARA MAIOR QUALIFICAÇÃO DAS AÇÕES DE CONTROLE, PORTANTOO PRIMEIRO EXERCÍCIO DE REFERÊNCIA SERÁ 2026.</t>
-        </is>
-      </c>
+      <c r="W233" t="inlineStr"/>
       <c r="X233" s="2" t="n">
         <v>45922.63333333333</v>
       </c>

</xml_diff>